<commit_message>
Hrs y Destajo Sem 26
</commit_message>
<xml_diff>
--- a/datasets/destajo.xlsx
+++ b/datasets/destajo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/275e1cc0366b6475/Documentos/Vori Vost/Pruebas-Boton/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{48AB0E75-7D41-47DC-B758-D10181A064D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E6D4DEB-FF72-4A8A-9650-D4BBC7932F74}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{48AB0E75-7D41-47DC-B758-D10181A064D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15CB91EB-D8AB-49D0-8764-FDB2FABB80CD}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{31EFA5F5-4BB3-40E1-95BE-59439A9739F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1888" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="114">
   <si>
     <t>SEMANA</t>
   </si>
@@ -364,6 +364,21 @@
   <si>
     <t>CTVV 2776 - Casa JML Primera Etapa - Miguel Maldonado</t>
   </si>
+  <si>
+    <t>Jesus Soto Días</t>
+  </si>
+  <si>
+    <t>CTVV 2592</t>
+  </si>
+  <si>
+    <t>CTVV 2592 - 6 CASAS TURIN 2A ETAPA- MEDA CASA</t>
+  </si>
+  <si>
+    <t>CTVV 3065</t>
+  </si>
+  <si>
+    <t>CTVV 3065 - Forrado de elevadores - Armando Chávez</t>
+  </si>
 </sst>
 </file>
 
@@ -435,13 +450,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}" name="Tabla3" displayName="Tabla3" ref="A1:V623" totalsRowShown="0">
-  <autoFilter ref="A1:V623" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}" name="Tabla3" displayName="Tabla3" ref="A1:V675" totalsRowShown="0">
+  <autoFilter ref="A1:V675" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}"/>
   <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{50CD881F-F4BE-4F9A-B2C3-50C2D8C2910F}" name="SEMANA"/>
     <tableColumn id="2" xr3:uid="{54EA7CC6-3702-4F53-8DD3-E9431860F33D}" name="PERÍODO"/>
@@ -787,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD62827-3B7E-49B3-B2B1-64E636F38ACC}">
-  <dimension ref="A1:V623"/>
+  <dimension ref="A1:V675"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A454" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F589" sqref="F589"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A647" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R651" sqref="R651"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -28283,6 +28294,2249 @@
         <v>2095.8274999999999</v>
       </c>
     </row>
+    <row r="624" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A624">
+        <v>26</v>
+      </c>
+      <c r="C624" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D624" t="s">
+        <v>62</v>
+      </c>
+      <c r="E624" t="s">
+        <v>95</v>
+      </c>
+      <c r="F624" t="s">
+        <v>96</v>
+      </c>
+      <c r="G624">
+        <v>3.52</v>
+      </c>
+      <c r="H624">
+        <v>700</v>
+      </c>
+      <c r="I624" s="2">
+        <v>2464</v>
+      </c>
+      <c r="J624">
+        <v>5</v>
+      </c>
+      <c r="K624">
+        <v>700</v>
+      </c>
+      <c r="L624" s="2">
+        <v>3500</v>
+      </c>
+      <c r="O624" s="2">
+        <v>0</v>
+      </c>
+      <c r="P624" s="2">
+        <v>5964</v>
+      </c>
+      <c r="S624" s="2">
+        <v>5964</v>
+      </c>
+      <c r="U624" s="2">
+        <v>5964</v>
+      </c>
+    </row>
+    <row r="625" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A625">
+        <v>26</v>
+      </c>
+      <c r="C625" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D625" t="s">
+        <v>62</v>
+      </c>
+      <c r="E625" t="s">
+        <v>95</v>
+      </c>
+      <c r="F625" t="s">
+        <v>96</v>
+      </c>
+      <c r="G625">
+        <v>1.84</v>
+      </c>
+      <c r="H625">
+        <v>700</v>
+      </c>
+      <c r="I625" s="2">
+        <v>1288</v>
+      </c>
+      <c r="J625">
+        <v>1</v>
+      </c>
+      <c r="K625">
+        <v>750</v>
+      </c>
+      <c r="L625" s="2">
+        <v>750</v>
+      </c>
+      <c r="O625" s="2">
+        <v>0</v>
+      </c>
+      <c r="P625" s="2">
+        <v>2038</v>
+      </c>
+      <c r="S625" s="2">
+        <v>2038</v>
+      </c>
+      <c r="U625" s="2">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="626" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A626">
+        <v>26</v>
+      </c>
+      <c r="C626" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D626" t="s">
+        <v>62</v>
+      </c>
+      <c r="E626" t="s">
+        <v>95</v>
+      </c>
+      <c r="F626" t="s">
+        <v>96</v>
+      </c>
+      <c r="G626">
+        <v>0.76</v>
+      </c>
+      <c r="H626">
+        <v>700</v>
+      </c>
+      <c r="I626" s="2">
+        <v>532</v>
+      </c>
+      <c r="L626" s="2">
+        <v>0</v>
+      </c>
+      <c r="O626" s="2">
+        <v>0</v>
+      </c>
+      <c r="P626" s="2">
+        <v>532</v>
+      </c>
+      <c r="Q626" s="2">
+        <v>500</v>
+      </c>
+      <c r="S626" s="2">
+        <v>1032</v>
+      </c>
+      <c r="U626" s="2">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="627" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A627">
+        <v>26</v>
+      </c>
+      <c r="C627" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D627" t="s">
+        <v>37</v>
+      </c>
+      <c r="E627" t="s">
+        <v>95</v>
+      </c>
+      <c r="F627" t="s">
+        <v>96</v>
+      </c>
+      <c r="G627">
+        <v>7.5</v>
+      </c>
+      <c r="H627">
+        <v>250</v>
+      </c>
+      <c r="I627" s="2">
+        <v>1875</v>
+      </c>
+      <c r="L627" s="2">
+        <v>0</v>
+      </c>
+      <c r="O627" s="2">
+        <v>0</v>
+      </c>
+      <c r="P627" s="2">
+        <v>1875</v>
+      </c>
+      <c r="S627" s="2">
+        <v>1875</v>
+      </c>
+      <c r="U627" s="2">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="628" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A628">
+        <v>26</v>
+      </c>
+      <c r="C628" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D628" t="s">
+        <v>37</v>
+      </c>
+      <c r="E628" t="s">
+        <v>95</v>
+      </c>
+      <c r="F628" t="s">
+        <v>96</v>
+      </c>
+      <c r="G628">
+        <v>3.71</v>
+      </c>
+      <c r="H628">
+        <v>700</v>
+      </c>
+      <c r="I628" s="2">
+        <v>2597</v>
+      </c>
+      <c r="L628" s="2">
+        <v>0</v>
+      </c>
+      <c r="O628" s="2">
+        <v>0</v>
+      </c>
+      <c r="P628" s="2">
+        <v>2597</v>
+      </c>
+      <c r="S628" s="2">
+        <v>2597</v>
+      </c>
+      <c r="U628" s="2">
+        <v>2597</v>
+      </c>
+    </row>
+    <row r="629" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A629">
+        <v>26</v>
+      </c>
+      <c r="C629" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D629" t="s">
+        <v>37</v>
+      </c>
+      <c r="E629" t="s">
+        <v>95</v>
+      </c>
+      <c r="F629" t="s">
+        <v>96</v>
+      </c>
+      <c r="G629">
+        <v>2.95</v>
+      </c>
+      <c r="H629">
+        <v>700</v>
+      </c>
+      <c r="I629" s="2">
+        <v>2065</v>
+      </c>
+      <c r="L629" s="2">
+        <v>0</v>
+      </c>
+      <c r="O629" s="2">
+        <v>0</v>
+      </c>
+      <c r="P629" s="2">
+        <v>2065</v>
+      </c>
+      <c r="S629" s="2">
+        <v>2065</v>
+      </c>
+      <c r="U629" s="2">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="630" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A630">
+        <v>26</v>
+      </c>
+      <c r="C630" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D630" t="s">
+        <v>37</v>
+      </c>
+      <c r="E630" t="s">
+        <v>95</v>
+      </c>
+      <c r="F630" t="s">
+        <v>96</v>
+      </c>
+      <c r="G630">
+        <v>2.95</v>
+      </c>
+      <c r="H630">
+        <v>700</v>
+      </c>
+      <c r="I630" s="2">
+        <v>2065</v>
+      </c>
+      <c r="L630" s="2">
+        <v>0</v>
+      </c>
+      <c r="O630" s="2">
+        <v>0</v>
+      </c>
+      <c r="P630" s="2">
+        <v>2065</v>
+      </c>
+      <c r="S630" s="2">
+        <v>2065</v>
+      </c>
+      <c r="U630" s="2">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="631" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A631">
+        <v>26</v>
+      </c>
+      <c r="C631" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D631" t="s">
+        <v>37</v>
+      </c>
+      <c r="E631" t="s">
+        <v>95</v>
+      </c>
+      <c r="F631" t="s">
+        <v>96</v>
+      </c>
+      <c r="I631" s="2">
+        <v>0</v>
+      </c>
+      <c r="J631">
+        <v>1</v>
+      </c>
+      <c r="K631">
+        <v>1800</v>
+      </c>
+      <c r="L631" s="2">
+        <v>1800</v>
+      </c>
+      <c r="O631" s="2">
+        <v>0</v>
+      </c>
+      <c r="P631" s="2">
+        <v>1800</v>
+      </c>
+      <c r="S631" s="2">
+        <v>1800</v>
+      </c>
+      <c r="U631" s="2">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="632" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A632">
+        <v>26</v>
+      </c>
+      <c r="C632" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D632" t="s">
+        <v>37</v>
+      </c>
+      <c r="E632" t="s">
+        <v>95</v>
+      </c>
+      <c r="F632" t="s">
+        <v>96</v>
+      </c>
+      <c r="I632" s="2">
+        <v>0</v>
+      </c>
+      <c r="J632">
+        <v>1</v>
+      </c>
+      <c r="K632">
+        <v>250</v>
+      </c>
+      <c r="L632" s="2">
+        <v>250</v>
+      </c>
+      <c r="O632" s="2">
+        <v>0</v>
+      </c>
+      <c r="P632" s="2">
+        <v>250</v>
+      </c>
+      <c r="S632" s="2">
+        <v>250</v>
+      </c>
+      <c r="U632" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="633" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A633">
+        <v>26</v>
+      </c>
+      <c r="C633" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D633" t="s">
+        <v>37</v>
+      </c>
+      <c r="E633" t="s">
+        <v>95</v>
+      </c>
+      <c r="F633" t="s">
+        <v>96</v>
+      </c>
+      <c r="I633" s="2">
+        <v>0</v>
+      </c>
+      <c r="J633">
+        <v>1</v>
+      </c>
+      <c r="K633">
+        <v>200</v>
+      </c>
+      <c r="L633" s="2">
+        <v>200</v>
+      </c>
+      <c r="O633" s="2">
+        <v>0</v>
+      </c>
+      <c r="P633" s="2">
+        <v>200</v>
+      </c>
+      <c r="S633" s="2">
+        <v>200</v>
+      </c>
+      <c r="U633" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="634" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A634">
+        <v>26</v>
+      </c>
+      <c r="C634" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D634" t="s">
+        <v>37</v>
+      </c>
+      <c r="E634" t="s">
+        <v>95</v>
+      </c>
+      <c r="F634" t="s">
+        <v>96</v>
+      </c>
+      <c r="I634" s="2">
+        <v>0</v>
+      </c>
+      <c r="J634">
+        <v>1</v>
+      </c>
+      <c r="K634">
+        <v>750</v>
+      </c>
+      <c r="L634" s="2">
+        <v>750</v>
+      </c>
+      <c r="O634" s="2">
+        <v>0</v>
+      </c>
+      <c r="P634" s="2">
+        <v>750</v>
+      </c>
+      <c r="S634" s="2">
+        <v>750</v>
+      </c>
+      <c r="U634" s="2">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="635" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A635">
+        <v>26</v>
+      </c>
+      <c r="C635" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D635" t="s">
+        <v>37</v>
+      </c>
+      <c r="E635" t="s">
+        <v>95</v>
+      </c>
+      <c r="F635" t="s">
+        <v>96</v>
+      </c>
+      <c r="I635" s="2">
+        <v>0</v>
+      </c>
+      <c r="J635">
+        <v>1</v>
+      </c>
+      <c r="K635">
+        <v>850</v>
+      </c>
+      <c r="L635" s="2">
+        <v>850</v>
+      </c>
+      <c r="O635" s="2">
+        <v>0</v>
+      </c>
+      <c r="P635" s="2">
+        <v>850</v>
+      </c>
+      <c r="S635" s="2">
+        <v>850</v>
+      </c>
+      <c r="U635" s="2">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="636" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A636">
+        <v>26</v>
+      </c>
+      <c r="C636" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D636" t="s">
+        <v>37</v>
+      </c>
+      <c r="E636" t="s">
+        <v>95</v>
+      </c>
+      <c r="F636" t="s">
+        <v>96</v>
+      </c>
+      <c r="G636">
+        <v>7.5</v>
+      </c>
+      <c r="H636">
+        <v>250</v>
+      </c>
+      <c r="I636" s="2">
+        <v>1875</v>
+      </c>
+      <c r="L636" s="2">
+        <v>0</v>
+      </c>
+      <c r="O636" s="2">
+        <v>0</v>
+      </c>
+      <c r="P636" s="2">
+        <v>1875</v>
+      </c>
+      <c r="Q636" s="2">
+        <v>500</v>
+      </c>
+      <c r="S636" s="2">
+        <v>2375</v>
+      </c>
+      <c r="U636" s="2">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="637" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A637">
+        <v>26</v>
+      </c>
+      <c r="C637" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D637" t="s">
+        <v>37</v>
+      </c>
+      <c r="E637" t="s">
+        <v>95</v>
+      </c>
+      <c r="F637" t="s">
+        <v>96</v>
+      </c>
+      <c r="I637" s="2">
+        <v>0</v>
+      </c>
+      <c r="L637" s="2">
+        <v>0</v>
+      </c>
+      <c r="M637">
+        <v>1</v>
+      </c>
+      <c r="N637">
+        <v>1083.33</v>
+      </c>
+      <c r="O637" s="2">
+        <v>1083.33</v>
+      </c>
+      <c r="P637" s="2">
+        <v>1083.33</v>
+      </c>
+      <c r="S637" s="2">
+        <v>1083.33</v>
+      </c>
+      <c r="U637" s="2">
+        <v>1083.33</v>
+      </c>
+    </row>
+    <row r="638" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A638">
+        <v>26</v>
+      </c>
+      <c r="C638" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D638" t="s">
+        <v>34</v>
+      </c>
+      <c r="E638" t="s">
+        <v>95</v>
+      </c>
+      <c r="F638" t="s">
+        <v>96</v>
+      </c>
+      <c r="G638">
+        <v>5.75</v>
+      </c>
+      <c r="H638">
+        <v>250</v>
+      </c>
+      <c r="I638" s="2">
+        <v>1437.5</v>
+      </c>
+      <c r="L638" s="2">
+        <v>0</v>
+      </c>
+      <c r="O638" s="2">
+        <v>0</v>
+      </c>
+      <c r="P638" s="2">
+        <v>1437.5</v>
+      </c>
+      <c r="S638" s="2">
+        <v>1437.5</v>
+      </c>
+      <c r="U638" s="2">
+        <v>1437.5</v>
+      </c>
+    </row>
+    <row r="639" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A639">
+        <v>26</v>
+      </c>
+      <c r="C639" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D639" t="s">
+        <v>34</v>
+      </c>
+      <c r="E639" t="s">
+        <v>95</v>
+      </c>
+      <c r="F639" t="s">
+        <v>96</v>
+      </c>
+      <c r="G639">
+        <v>2.36</v>
+      </c>
+      <c r="H639">
+        <v>700</v>
+      </c>
+      <c r="I639" s="2">
+        <v>1652</v>
+      </c>
+      <c r="J639">
+        <v>5</v>
+      </c>
+      <c r="K639">
+        <v>700</v>
+      </c>
+      <c r="L639" s="2">
+        <v>3500</v>
+      </c>
+      <c r="O639" s="2">
+        <v>0</v>
+      </c>
+      <c r="P639" s="2">
+        <v>5152</v>
+      </c>
+      <c r="S639" s="2">
+        <v>5152</v>
+      </c>
+      <c r="U639" s="2">
+        <v>5152</v>
+      </c>
+    </row>
+    <row r="640" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A640">
+        <v>26</v>
+      </c>
+      <c r="C640" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D640" t="s">
+        <v>34</v>
+      </c>
+      <c r="E640" t="s">
+        <v>95</v>
+      </c>
+      <c r="F640" t="s">
+        <v>96</v>
+      </c>
+      <c r="G640">
+        <v>3.68</v>
+      </c>
+      <c r="H640">
+        <v>250</v>
+      </c>
+      <c r="I640" s="2">
+        <v>920</v>
+      </c>
+      <c r="L640" s="2">
+        <v>0</v>
+      </c>
+      <c r="O640" s="2">
+        <v>0</v>
+      </c>
+      <c r="P640" s="2">
+        <v>920</v>
+      </c>
+      <c r="Q640" s="2">
+        <v>500</v>
+      </c>
+      <c r="S640" s="2">
+        <v>1420</v>
+      </c>
+      <c r="U640" s="2">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="641" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A641">
+        <v>26</v>
+      </c>
+      <c r="C641" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D641" t="s">
+        <v>56</v>
+      </c>
+      <c r="E641" t="s">
+        <v>76</v>
+      </c>
+      <c r="F641" t="s">
+        <v>77</v>
+      </c>
+      <c r="G641">
+        <v>0.72</v>
+      </c>
+      <c r="H641">
+        <v>500</v>
+      </c>
+      <c r="I641" s="2">
+        <v>360</v>
+      </c>
+      <c r="L641" s="2">
+        <v>0</v>
+      </c>
+      <c r="O641" s="2">
+        <v>0</v>
+      </c>
+      <c r="P641" s="2">
+        <v>360</v>
+      </c>
+      <c r="S641" s="2">
+        <v>360</v>
+      </c>
+      <c r="U641" s="2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="642" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A642">
+        <v>26</v>
+      </c>
+      <c r="C642" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D642" t="s">
+        <v>56</v>
+      </c>
+      <c r="E642" t="s">
+        <v>76</v>
+      </c>
+      <c r="F642" t="s">
+        <v>77</v>
+      </c>
+      <c r="G642">
+        <v>6.11</v>
+      </c>
+      <c r="H642">
+        <v>750</v>
+      </c>
+      <c r="I642" s="2">
+        <v>4582.5</v>
+      </c>
+      <c r="L642" s="2">
+        <v>0</v>
+      </c>
+      <c r="O642" s="2">
+        <v>0</v>
+      </c>
+      <c r="P642" s="2">
+        <v>4582.5</v>
+      </c>
+      <c r="S642" s="2">
+        <v>4582.5</v>
+      </c>
+      <c r="U642" s="2">
+        <v>4582.5</v>
+      </c>
+    </row>
+    <row r="643" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A643">
+        <v>26</v>
+      </c>
+      <c r="C643" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D643" t="s">
+        <v>56</v>
+      </c>
+      <c r="E643" t="s">
+        <v>76</v>
+      </c>
+      <c r="F643" t="s">
+        <v>77</v>
+      </c>
+      <c r="G643">
+        <v>5.2</v>
+      </c>
+      <c r="H643">
+        <v>400</v>
+      </c>
+      <c r="I643" s="2">
+        <v>2080</v>
+      </c>
+      <c r="L643" s="2">
+        <v>0</v>
+      </c>
+      <c r="O643" s="2">
+        <v>0</v>
+      </c>
+      <c r="P643" s="2">
+        <v>2080</v>
+      </c>
+      <c r="Q643" s="2">
+        <v>500</v>
+      </c>
+      <c r="S643" s="2">
+        <v>2580</v>
+      </c>
+      <c r="U643" s="2">
+        <v>2580</v>
+      </c>
+    </row>
+    <row r="644" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A644">
+        <v>26</v>
+      </c>
+      <c r="C644" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D644" t="s">
+        <v>78</v>
+      </c>
+      <c r="E644" t="s">
+        <v>79</v>
+      </c>
+      <c r="F644" t="s">
+        <v>80</v>
+      </c>
+      <c r="G644">
+        <v>2.1905000000000001</v>
+      </c>
+      <c r="H644">
+        <v>400</v>
+      </c>
+      <c r="I644" s="2">
+        <v>876.2</v>
+      </c>
+      <c r="J644">
+        <v>1</v>
+      </c>
+      <c r="K644">
+        <v>300</v>
+      </c>
+      <c r="L644" s="2">
+        <v>300</v>
+      </c>
+      <c r="M644">
+        <v>1</v>
+      </c>
+      <c r="N644">
+        <v>1083.33</v>
+      </c>
+      <c r="O644" s="2">
+        <v>1083.33</v>
+      </c>
+      <c r="P644" s="2">
+        <v>2259.5299999999997</v>
+      </c>
+      <c r="S644" s="2">
+        <v>2259.5299999999997</v>
+      </c>
+      <c r="U644" s="2">
+        <v>2259.5299999999997</v>
+      </c>
+    </row>
+    <row r="645" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A645">
+        <v>26</v>
+      </c>
+      <c r="C645" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D645" t="s">
+        <v>78</v>
+      </c>
+      <c r="E645" t="s">
+        <v>79</v>
+      </c>
+      <c r="F645" t="s">
+        <v>80</v>
+      </c>
+      <c r="G645">
+        <v>4.3810000000000002</v>
+      </c>
+      <c r="H645">
+        <v>250</v>
+      </c>
+      <c r="I645" s="2">
+        <v>1095.25</v>
+      </c>
+      <c r="L645" s="2">
+        <v>0</v>
+      </c>
+      <c r="M645">
+        <v>0.75</v>
+      </c>
+      <c r="N645">
+        <v>1083.33</v>
+      </c>
+      <c r="O645" s="2">
+        <v>812.49749999999995</v>
+      </c>
+      <c r="P645" s="2">
+        <v>1907.7474999999999</v>
+      </c>
+      <c r="S645" s="2">
+        <v>1907.7474999999999</v>
+      </c>
+      <c r="U645" s="2">
+        <v>1907.7474999999999</v>
+      </c>
+    </row>
+    <row r="646" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A646">
+        <v>26</v>
+      </c>
+      <c r="C646" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D646" t="s">
+        <v>78</v>
+      </c>
+      <c r="E646" t="s">
+        <v>79</v>
+      </c>
+      <c r="F646" t="s">
+        <v>80</v>
+      </c>
+      <c r="I646" s="2">
+        <v>0</v>
+      </c>
+      <c r="L646" s="2">
+        <v>0</v>
+      </c>
+      <c r="M646">
+        <v>0.35</v>
+      </c>
+      <c r="N646">
+        <v>1083.33</v>
+      </c>
+      <c r="O646" s="2">
+        <v>379.16549999999995</v>
+      </c>
+      <c r="P646" s="2">
+        <v>379.16549999999995</v>
+      </c>
+      <c r="S646" s="2">
+        <v>379.16549999999995</v>
+      </c>
+      <c r="U646" s="2">
+        <v>379.16549999999995</v>
+      </c>
+    </row>
+    <row r="647" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A647">
+        <v>26</v>
+      </c>
+      <c r="C647" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D647" t="s">
+        <v>78</v>
+      </c>
+      <c r="E647" t="s">
+        <v>79</v>
+      </c>
+      <c r="F647" t="s">
+        <v>80</v>
+      </c>
+      <c r="I647" s="2">
+        <v>0</v>
+      </c>
+      <c r="L647" s="2">
+        <v>0</v>
+      </c>
+      <c r="M647">
+        <v>0.35</v>
+      </c>
+      <c r="N647">
+        <v>1083.33</v>
+      </c>
+      <c r="O647" s="2">
+        <v>379.16549999999995</v>
+      </c>
+      <c r="P647" s="2">
+        <v>379.16549999999995</v>
+      </c>
+      <c r="Q647" s="2">
+        <v>500</v>
+      </c>
+      <c r="S647" s="2">
+        <v>879.16549999999995</v>
+      </c>
+      <c r="U647" s="2">
+        <v>879.16549999999995</v>
+      </c>
+    </row>
+    <row r="648" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A648">
+        <v>26</v>
+      </c>
+      <c r="C648" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D648" t="s">
+        <v>38</v>
+      </c>
+      <c r="E648" t="s">
+        <v>107</v>
+      </c>
+      <c r="F648" t="s">
+        <v>108</v>
+      </c>
+      <c r="G648">
+        <v>1.5</v>
+      </c>
+      <c r="H648">
+        <v>800</v>
+      </c>
+      <c r="I648" s="2">
+        <v>1200</v>
+      </c>
+      <c r="L648" s="2">
+        <v>0</v>
+      </c>
+      <c r="O648" s="2">
+        <v>0</v>
+      </c>
+      <c r="P648" s="2">
+        <v>1200</v>
+      </c>
+      <c r="S648" s="2">
+        <v>1200</v>
+      </c>
+      <c r="U648" s="2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="649" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A649">
+        <v>26</v>
+      </c>
+      <c r="C649" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D649" t="s">
+        <v>53</v>
+      </c>
+      <c r="E649" t="s">
+        <v>107</v>
+      </c>
+      <c r="F649" t="s">
+        <v>108</v>
+      </c>
+      <c r="I649" s="2">
+        <v>0</v>
+      </c>
+      <c r="J649">
+        <v>1</v>
+      </c>
+      <c r="K649">
+        <v>1200</v>
+      </c>
+      <c r="L649" s="2">
+        <v>1200</v>
+      </c>
+      <c r="O649" s="2">
+        <v>0</v>
+      </c>
+      <c r="P649" s="2">
+        <v>1200</v>
+      </c>
+      <c r="Q649" s="2">
+        <v>100</v>
+      </c>
+      <c r="S649" s="2">
+        <v>1300</v>
+      </c>
+      <c r="U649" s="2">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="650" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A650">
+        <v>26</v>
+      </c>
+      <c r="C650" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D650" t="s">
+        <v>109</v>
+      </c>
+      <c r="E650" t="s">
+        <v>110</v>
+      </c>
+      <c r="F650" t="s">
+        <v>111</v>
+      </c>
+      <c r="G650">
+        <v>2.83</v>
+      </c>
+      <c r="H650">
+        <v>700</v>
+      </c>
+      <c r="I650" s="2">
+        <v>1981</v>
+      </c>
+      <c r="L650" s="2">
+        <v>0</v>
+      </c>
+      <c r="O650" s="2">
+        <v>0</v>
+      </c>
+      <c r="P650" s="2">
+        <v>1981</v>
+      </c>
+      <c r="S650" s="2">
+        <v>1981</v>
+      </c>
+      <c r="U650" s="2">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="651" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A651">
+        <v>26</v>
+      </c>
+      <c r="C651" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D651" t="s">
+        <v>29</v>
+      </c>
+      <c r="E651" t="s">
+        <v>84</v>
+      </c>
+      <c r="F651" t="s">
+        <v>85</v>
+      </c>
+      <c r="I651" s="2">
+        <v>0</v>
+      </c>
+      <c r="J651">
+        <v>1</v>
+      </c>
+      <c r="K651">
+        <v>150</v>
+      </c>
+      <c r="L651" s="2">
+        <v>150</v>
+      </c>
+      <c r="O651" s="2">
+        <v>0</v>
+      </c>
+      <c r="P651" s="2">
+        <v>150</v>
+      </c>
+      <c r="S651" s="2">
+        <v>150</v>
+      </c>
+      <c r="U651" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="652" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A652">
+        <v>26</v>
+      </c>
+      <c r="C652" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D652" t="s">
+        <v>29</v>
+      </c>
+      <c r="E652" t="s">
+        <v>84</v>
+      </c>
+      <c r="F652" t="s">
+        <v>85</v>
+      </c>
+      <c r="I652" s="2">
+        <v>0</v>
+      </c>
+      <c r="J652">
+        <v>1</v>
+      </c>
+      <c r="K652">
+        <v>150</v>
+      </c>
+      <c r="L652" s="2">
+        <v>150</v>
+      </c>
+      <c r="O652" s="2">
+        <v>0</v>
+      </c>
+      <c r="P652" s="2">
+        <v>150</v>
+      </c>
+      <c r="S652" s="2">
+        <v>150</v>
+      </c>
+      <c r="U652" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="653" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A653">
+        <v>26</v>
+      </c>
+      <c r="C653" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D653" t="s">
+        <v>29</v>
+      </c>
+      <c r="E653" t="s">
+        <v>84</v>
+      </c>
+      <c r="F653" t="s">
+        <v>85</v>
+      </c>
+      <c r="I653" s="2">
+        <v>0</v>
+      </c>
+      <c r="J653">
+        <v>1</v>
+      </c>
+      <c r="K653">
+        <v>150</v>
+      </c>
+      <c r="L653" s="2">
+        <v>150</v>
+      </c>
+      <c r="O653" s="2">
+        <v>0</v>
+      </c>
+      <c r="P653" s="2">
+        <v>150</v>
+      </c>
+      <c r="S653" s="2">
+        <v>150</v>
+      </c>
+      <c r="U653" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="654" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A654">
+        <v>26</v>
+      </c>
+      <c r="C654" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D654" t="s">
+        <v>29</v>
+      </c>
+      <c r="E654" t="s">
+        <v>84</v>
+      </c>
+      <c r="F654" t="s">
+        <v>85</v>
+      </c>
+      <c r="I654" s="2">
+        <v>0</v>
+      </c>
+      <c r="J654">
+        <v>1</v>
+      </c>
+      <c r="K654">
+        <v>150</v>
+      </c>
+      <c r="L654" s="2">
+        <v>150</v>
+      </c>
+      <c r="O654" s="2">
+        <v>0</v>
+      </c>
+      <c r="P654" s="2">
+        <v>150</v>
+      </c>
+      <c r="S654" s="2">
+        <v>150</v>
+      </c>
+      <c r="U654" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="655" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A655">
+        <v>26</v>
+      </c>
+      <c r="C655" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D655" t="s">
+        <v>29</v>
+      </c>
+      <c r="E655" t="s">
+        <v>84</v>
+      </c>
+      <c r="F655" t="s">
+        <v>85</v>
+      </c>
+      <c r="I655" s="2">
+        <v>0</v>
+      </c>
+      <c r="J655">
+        <v>1</v>
+      </c>
+      <c r="K655">
+        <v>150</v>
+      </c>
+      <c r="L655" s="2">
+        <v>150</v>
+      </c>
+      <c r="O655" s="2">
+        <v>0</v>
+      </c>
+      <c r="P655" s="2">
+        <v>150</v>
+      </c>
+      <c r="S655" s="2">
+        <v>150</v>
+      </c>
+      <c r="U655" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="656" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A656">
+        <v>26</v>
+      </c>
+      <c r="C656" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D656" t="s">
+        <v>29</v>
+      </c>
+      <c r="E656" t="s">
+        <v>84</v>
+      </c>
+      <c r="F656" t="s">
+        <v>85</v>
+      </c>
+      <c r="I656" s="2">
+        <v>0</v>
+      </c>
+      <c r="J656">
+        <v>1</v>
+      </c>
+      <c r="K656">
+        <v>150</v>
+      </c>
+      <c r="L656" s="2">
+        <v>150</v>
+      </c>
+      <c r="O656" s="2">
+        <v>0</v>
+      </c>
+      <c r="P656" s="2">
+        <v>150</v>
+      </c>
+      <c r="Q656" s="2">
+        <v>200</v>
+      </c>
+      <c r="S656" s="2">
+        <v>350</v>
+      </c>
+      <c r="U656" s="2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="657" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A657">
+        <v>26</v>
+      </c>
+      <c r="C657" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D657" t="s">
+        <v>22</v>
+      </c>
+      <c r="E657" t="s">
+        <v>23</v>
+      </c>
+      <c r="F657" t="s">
+        <v>24</v>
+      </c>
+      <c r="I657" s="2">
+        <v>0</v>
+      </c>
+      <c r="J657">
+        <v>10</v>
+      </c>
+      <c r="K657">
+        <v>140</v>
+      </c>
+      <c r="L657" s="2">
+        <v>1400</v>
+      </c>
+      <c r="O657" s="2">
+        <v>0</v>
+      </c>
+      <c r="P657" s="2">
+        <v>1400</v>
+      </c>
+      <c r="S657" s="2">
+        <v>1400</v>
+      </c>
+      <c r="U657" s="2">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="658" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A658">
+        <v>26</v>
+      </c>
+      <c r="C658" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D658" t="s">
+        <v>41</v>
+      </c>
+      <c r="E658" t="s">
+        <v>105</v>
+      </c>
+      <c r="F658" t="s">
+        <v>106</v>
+      </c>
+      <c r="G658">
+        <v>1.17</v>
+      </c>
+      <c r="H658">
+        <v>700</v>
+      </c>
+      <c r="I658" s="2">
+        <v>819</v>
+      </c>
+      <c r="J658">
+        <v>1</v>
+      </c>
+      <c r="K658">
+        <v>500</v>
+      </c>
+      <c r="L658" s="2">
+        <v>500</v>
+      </c>
+      <c r="O658" s="2">
+        <v>0</v>
+      </c>
+      <c r="P658" s="2">
+        <v>1319</v>
+      </c>
+      <c r="S658" s="2">
+        <v>1319</v>
+      </c>
+      <c r="U658" s="2">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="659" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A659">
+        <v>26</v>
+      </c>
+      <c r="C659" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D659" t="s">
+        <v>41</v>
+      </c>
+      <c r="E659" t="s">
+        <v>105</v>
+      </c>
+      <c r="F659" t="s">
+        <v>106</v>
+      </c>
+      <c r="G659">
+        <v>1.95</v>
+      </c>
+      <c r="H659">
+        <v>300</v>
+      </c>
+      <c r="I659" s="2">
+        <v>585</v>
+      </c>
+      <c r="L659" s="2">
+        <v>0</v>
+      </c>
+      <c r="O659" s="2">
+        <v>0</v>
+      </c>
+      <c r="P659" s="2">
+        <v>585</v>
+      </c>
+      <c r="S659" s="2">
+        <v>585</v>
+      </c>
+      <c r="U659" s="2">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="660" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A660">
+        <v>26</v>
+      </c>
+      <c r="C660" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D660" t="s">
+        <v>59</v>
+      </c>
+      <c r="E660" t="s">
+        <v>105</v>
+      </c>
+      <c r="F660" t="s">
+        <v>106</v>
+      </c>
+      <c r="G660">
+        <v>1.17</v>
+      </c>
+      <c r="H660">
+        <v>700</v>
+      </c>
+      <c r="I660" s="2">
+        <v>819</v>
+      </c>
+      <c r="L660" s="2">
+        <v>0</v>
+      </c>
+      <c r="O660" s="2">
+        <v>0</v>
+      </c>
+      <c r="P660" s="2">
+        <v>819</v>
+      </c>
+      <c r="S660" s="2">
+        <v>819</v>
+      </c>
+      <c r="U660" s="2">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="661" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A661">
+        <v>26</v>
+      </c>
+      <c r="C661" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D661" t="s">
+        <v>59</v>
+      </c>
+      <c r="E661" t="s">
+        <v>105</v>
+      </c>
+      <c r="F661" t="s">
+        <v>106</v>
+      </c>
+      <c r="G661">
+        <v>1.95</v>
+      </c>
+      <c r="H661">
+        <v>300</v>
+      </c>
+      <c r="I661" s="2">
+        <v>585</v>
+      </c>
+      <c r="L661" s="2">
+        <v>0</v>
+      </c>
+      <c r="O661" s="2">
+        <v>0</v>
+      </c>
+      <c r="P661" s="2">
+        <v>585</v>
+      </c>
+      <c r="S661" s="2">
+        <v>585</v>
+      </c>
+      <c r="U661" s="2">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="662" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A662">
+        <v>26</v>
+      </c>
+      <c r="C662" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D662" t="s">
+        <v>81</v>
+      </c>
+      <c r="E662" t="s">
+        <v>105</v>
+      </c>
+      <c r="F662" t="s">
+        <v>106</v>
+      </c>
+      <c r="G662">
+        <v>2.34</v>
+      </c>
+      <c r="H662">
+        <v>700</v>
+      </c>
+      <c r="I662" s="2">
+        <v>1638</v>
+      </c>
+      <c r="J662">
+        <v>1</v>
+      </c>
+      <c r="K662">
+        <v>250</v>
+      </c>
+      <c r="L662" s="2">
+        <v>250</v>
+      </c>
+      <c r="O662" s="2">
+        <v>0</v>
+      </c>
+      <c r="P662" s="2">
+        <v>1888</v>
+      </c>
+      <c r="S662" s="2">
+        <v>1888</v>
+      </c>
+      <c r="U662" s="2">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="663" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A663">
+        <v>26</v>
+      </c>
+      <c r="C663" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D663" t="s">
+        <v>81</v>
+      </c>
+      <c r="E663" t="s">
+        <v>105</v>
+      </c>
+      <c r="F663" t="s">
+        <v>106</v>
+      </c>
+      <c r="G663">
+        <v>2.4</v>
+      </c>
+      <c r="H663">
+        <v>300</v>
+      </c>
+      <c r="I663" s="2">
+        <v>720</v>
+      </c>
+      <c r="J663">
+        <v>1</v>
+      </c>
+      <c r="K663">
+        <v>200</v>
+      </c>
+      <c r="L663" s="2">
+        <v>200</v>
+      </c>
+      <c r="O663" s="2">
+        <v>0</v>
+      </c>
+      <c r="P663" s="2">
+        <v>920</v>
+      </c>
+      <c r="S663" s="2">
+        <v>920</v>
+      </c>
+      <c r="U663" s="2">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="664" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A664">
+        <v>26</v>
+      </c>
+      <c r="C664" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D664" t="s">
+        <v>81</v>
+      </c>
+      <c r="E664" t="s">
+        <v>105</v>
+      </c>
+      <c r="F664" t="s">
+        <v>106</v>
+      </c>
+      <c r="G664">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="H664">
+        <v>700</v>
+      </c>
+      <c r="I664" s="2">
+        <v>647.5</v>
+      </c>
+      <c r="J664">
+        <v>1</v>
+      </c>
+      <c r="K664">
+        <v>200</v>
+      </c>
+      <c r="L664" s="2">
+        <v>200</v>
+      </c>
+      <c r="O664" s="2">
+        <v>0</v>
+      </c>
+      <c r="P664" s="2">
+        <v>847.5</v>
+      </c>
+      <c r="S664" s="2">
+        <v>847.5</v>
+      </c>
+      <c r="U664" s="2">
+        <v>847.5</v>
+      </c>
+    </row>
+    <row r="665" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A665">
+        <v>26</v>
+      </c>
+      <c r="C665" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D665" t="s">
+        <v>81</v>
+      </c>
+      <c r="E665" t="s">
+        <v>105</v>
+      </c>
+      <c r="F665" t="s">
+        <v>106</v>
+      </c>
+      <c r="G665">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="H665">
+        <v>700</v>
+      </c>
+      <c r="I665" s="2">
+        <v>549.5</v>
+      </c>
+      <c r="L665" s="2">
+        <v>0</v>
+      </c>
+      <c r="O665" s="2">
+        <v>0</v>
+      </c>
+      <c r="P665" s="2">
+        <v>549.5</v>
+      </c>
+      <c r="S665" s="2">
+        <v>549.5</v>
+      </c>
+      <c r="U665" s="2">
+        <v>549.5</v>
+      </c>
+    </row>
+    <row r="666" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A666">
+        <v>26</v>
+      </c>
+      <c r="C666" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D666" t="s">
+        <v>81</v>
+      </c>
+      <c r="E666" t="s">
+        <v>105</v>
+      </c>
+      <c r="F666" t="s">
+        <v>106</v>
+      </c>
+      <c r="G666">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="H666">
+        <v>700</v>
+      </c>
+      <c r="I666" s="2">
+        <v>647.5</v>
+      </c>
+      <c r="L666" s="2">
+        <v>0</v>
+      </c>
+      <c r="O666" s="2">
+        <v>0</v>
+      </c>
+      <c r="P666" s="2">
+        <v>647.5</v>
+      </c>
+      <c r="S666" s="2">
+        <v>647.5</v>
+      </c>
+      <c r="U666" s="2">
+        <v>647.5</v>
+      </c>
+    </row>
+    <row r="667" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A667">
+        <v>26</v>
+      </c>
+      <c r="C667" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D667" t="s">
+        <v>81</v>
+      </c>
+      <c r="E667" t="s">
+        <v>105</v>
+      </c>
+      <c r="F667" t="s">
+        <v>106</v>
+      </c>
+      <c r="G667">
+        <v>0.73</v>
+      </c>
+      <c r="H667">
+        <v>700</v>
+      </c>
+      <c r="I667" s="2">
+        <v>511</v>
+      </c>
+      <c r="L667" s="2">
+        <v>0</v>
+      </c>
+      <c r="O667" s="2">
+        <v>0</v>
+      </c>
+      <c r="P667" s="2">
+        <v>511</v>
+      </c>
+      <c r="Q667" s="2">
+        <v>500</v>
+      </c>
+      <c r="S667" s="2">
+        <v>1011</v>
+      </c>
+      <c r="U667" s="2">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="668" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A668">
+        <v>26</v>
+      </c>
+      <c r="C668" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D668" t="s">
+        <v>34</v>
+      </c>
+      <c r="E668" t="s">
+        <v>84</v>
+      </c>
+      <c r="F668" t="s">
+        <v>85</v>
+      </c>
+      <c r="G668">
+        <v>2</v>
+      </c>
+      <c r="H668">
+        <v>700</v>
+      </c>
+      <c r="I668" s="2">
+        <v>1400</v>
+      </c>
+      <c r="L668" s="2">
+        <v>0</v>
+      </c>
+      <c r="O668" s="2">
+        <v>0</v>
+      </c>
+      <c r="P668" s="2">
+        <v>1400</v>
+      </c>
+      <c r="S668" s="2">
+        <v>1400</v>
+      </c>
+      <c r="U668" s="2">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="669" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A669">
+        <v>26</v>
+      </c>
+      <c r="C669" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D669" t="s">
+        <v>34</v>
+      </c>
+      <c r="E669" t="s">
+        <v>84</v>
+      </c>
+      <c r="F669" t="s">
+        <v>85</v>
+      </c>
+      <c r="G669">
+        <v>2</v>
+      </c>
+      <c r="H669">
+        <v>700</v>
+      </c>
+      <c r="I669" s="2">
+        <v>1400</v>
+      </c>
+      <c r="L669" s="2">
+        <v>0</v>
+      </c>
+      <c r="O669" s="2">
+        <v>0</v>
+      </c>
+      <c r="P669" s="2">
+        <v>1400</v>
+      </c>
+      <c r="S669" s="2">
+        <v>1400</v>
+      </c>
+      <c r="U669" s="2">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="670" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A670">
+        <v>26</v>
+      </c>
+      <c r="C670" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D670" t="s">
+        <v>44</v>
+      </c>
+      <c r="E670" t="s">
+        <v>39</v>
+      </c>
+      <c r="F670" t="s">
+        <v>40</v>
+      </c>
+      <c r="I670" s="2">
+        <v>0</v>
+      </c>
+      <c r="L670" s="2">
+        <v>0</v>
+      </c>
+      <c r="M670">
+        <v>0.65</v>
+      </c>
+      <c r="N670">
+        <v>1083.33</v>
+      </c>
+      <c r="O670" s="2">
+        <v>704.16449999999998</v>
+      </c>
+      <c r="P670" s="2">
+        <v>704.16449999999998</v>
+      </c>
+      <c r="S670" s="2">
+        <v>704.16449999999998</v>
+      </c>
+      <c r="U670" s="2">
+        <v>704.16449999999998</v>
+      </c>
+    </row>
+    <row r="671" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A671">
+        <v>26</v>
+      </c>
+      <c r="C671" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D671" t="s">
+        <v>44</v>
+      </c>
+      <c r="E671" t="s">
+        <v>39</v>
+      </c>
+      <c r="F671" t="s">
+        <v>40</v>
+      </c>
+      <c r="I671" s="2">
+        <v>0</v>
+      </c>
+      <c r="L671" s="2">
+        <v>0</v>
+      </c>
+      <c r="M671">
+        <v>0.5</v>
+      </c>
+      <c r="N671">
+        <v>1083.33</v>
+      </c>
+      <c r="O671" s="2">
+        <v>541.66499999999996</v>
+      </c>
+      <c r="P671" s="2">
+        <v>541.66499999999996</v>
+      </c>
+      <c r="Q671" s="2">
+        <v>100</v>
+      </c>
+      <c r="S671" s="2">
+        <v>641.66499999999996</v>
+      </c>
+      <c r="U671" s="2">
+        <v>641.66499999999996</v>
+      </c>
+    </row>
+    <row r="672" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A672">
+        <v>26</v>
+      </c>
+      <c r="C672" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D672" t="s">
+        <v>48</v>
+      </c>
+      <c r="E672" t="s">
+        <v>105</v>
+      </c>
+      <c r="F672" t="s">
+        <v>106</v>
+      </c>
+      <c r="G672">
+        <v>2.96</v>
+      </c>
+      <c r="H672">
+        <v>700</v>
+      </c>
+      <c r="I672" s="2">
+        <v>2072</v>
+      </c>
+      <c r="J672">
+        <v>1</v>
+      </c>
+      <c r="K672">
+        <v>200</v>
+      </c>
+      <c r="L672" s="2">
+        <v>200</v>
+      </c>
+      <c r="O672" s="2">
+        <v>0</v>
+      </c>
+      <c r="P672" s="2">
+        <v>2272</v>
+      </c>
+      <c r="S672" s="2">
+        <v>2272</v>
+      </c>
+      <c r="U672" s="2">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="673" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A673">
+        <v>26</v>
+      </c>
+      <c r="C673" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D673" t="s">
+        <v>48</v>
+      </c>
+      <c r="E673" t="s">
+        <v>105</v>
+      </c>
+      <c r="F673" t="s">
+        <v>106</v>
+      </c>
+      <c r="G673">
+        <v>1.74</v>
+      </c>
+      <c r="H673">
+        <v>700</v>
+      </c>
+      <c r="I673" s="2">
+        <v>1218</v>
+      </c>
+      <c r="J673">
+        <v>1</v>
+      </c>
+      <c r="K673">
+        <v>200</v>
+      </c>
+      <c r="L673" s="2">
+        <v>200</v>
+      </c>
+      <c r="O673" s="2">
+        <v>0</v>
+      </c>
+      <c r="P673" s="2">
+        <v>1418</v>
+      </c>
+      <c r="S673" s="2">
+        <v>1418</v>
+      </c>
+      <c r="U673" s="2">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="674" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A674">
+        <v>26</v>
+      </c>
+      <c r="C674" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D674" t="s">
+        <v>48</v>
+      </c>
+      <c r="E674" t="s">
+        <v>105</v>
+      </c>
+      <c r="F674" t="s">
+        <v>106</v>
+      </c>
+      <c r="G674">
+        <v>1.66</v>
+      </c>
+      <c r="H674">
+        <v>700</v>
+      </c>
+      <c r="I674" s="2">
+        <v>1162</v>
+      </c>
+      <c r="J674">
+        <v>1</v>
+      </c>
+      <c r="K674">
+        <v>200</v>
+      </c>
+      <c r="L674" s="2">
+        <v>200</v>
+      </c>
+      <c r="O674" s="2">
+        <v>0</v>
+      </c>
+      <c r="P674" s="2">
+        <v>1362</v>
+      </c>
+      <c r="Q674" s="2">
+        <v>500</v>
+      </c>
+      <c r="S674" s="2">
+        <v>1862</v>
+      </c>
+      <c r="U674" s="2">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="675" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A675">
+        <v>26</v>
+      </c>
+      <c r="C675" s="1">
+        <v>45470</v>
+      </c>
+      <c r="D675" t="s">
+        <v>59</v>
+      </c>
+      <c r="E675" t="s">
+        <v>112</v>
+      </c>
+      <c r="F675" t="s">
+        <v>113</v>
+      </c>
+      <c r="I675" s="2">
+        <v>0</v>
+      </c>
+      <c r="L675" s="2">
+        <v>0</v>
+      </c>
+      <c r="M675">
+        <v>2</v>
+      </c>
+      <c r="N675">
+        <v>750</v>
+      </c>
+      <c r="O675" s="2">
+        <v>1500</v>
+      </c>
+      <c r="P675" s="2">
+        <v>1500</v>
+      </c>
+      <c r="Q675" s="2">
+        <v>100</v>
+      </c>
+      <c r="S675" s="2">
+        <v>1600</v>
+      </c>
+      <c r="U675" s="2">
+        <v>1600</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Destajo Hrs Extras Sem 37
</commit_message>
<xml_diff>
--- a/datasets/destajo.xlsx
+++ b/datasets/destajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/275e1cc0366b6475/Documentos/Vori Vost/Pruebas-Boton/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{48AB0E75-7D41-47DC-B758-D10181A064D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08FE5F97-3760-4DD0-AD5C-164592EF62A0}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{48AB0E75-7D41-47DC-B758-D10181A064D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67FCFB52-4134-40DE-97AC-0B36385E13F5}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{31EFA5F5-4BB3-40E1-95BE-59439A9739F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3136" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3256" uniqueCount="134">
   <si>
     <t>SEMANA</t>
   </si>
@@ -427,6 +427,18 @@
   <si>
     <t>CTVV 3092 - Remodelación Casa Mata - José Luis Ramírez</t>
   </si>
+  <si>
+    <t>CTVV 3078</t>
+  </si>
+  <si>
+    <t>CTVV 3078 - Piso 5 Centro Capital Oficina 02 LN - Canaco</t>
+  </si>
+  <si>
+    <t>CTVV 1176</t>
+  </si>
+  <si>
+    <t>CTVV 1176 - CASA ANDREA SANCHEZ - ANDREA SANCHEZ</t>
+  </si>
 </sst>
 </file>
 
@@ -498,9 +510,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}" name="Tabla3" displayName="Tabla3" ref="A1:V1039" totalsRowShown="0">
-  <autoFilter ref="A1:V1039" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}" name="Tabla3" displayName="Tabla3" ref="A1:V1079" totalsRowShown="0">
+  <autoFilter ref="A1:V1079" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}"/>
   <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{50CD881F-F4BE-4F9A-B2C3-50C2D8C2910F}" name="SEMANA"/>
     <tableColumn id="2" xr3:uid="{54EA7CC6-3702-4F53-8DD3-E9431860F33D}" name="PERÍODO"/>
@@ -846,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD62827-3B7E-49B3-B2B1-64E636F38ACC}">
-  <dimension ref="A1:V1039"/>
+  <dimension ref="A1:V1079"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A985" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F998" sqref="F998"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1057" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1069" sqref="F1069"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -46505,6 +46521,1754 @@
         <v>8312</v>
       </c>
     </row>
+    <row r="1040" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1040">
+        <v>37</v>
+      </c>
+      <c r="C1040" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1040" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1040" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1040" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1040">
+        <v>3.25</v>
+      </c>
+      <c r="H1040">
+        <v>200</v>
+      </c>
+      <c r="I1040" s="2">
+        <v>650</v>
+      </c>
+      <c r="L1040" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1040" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1040" s="2">
+        <v>650</v>
+      </c>
+      <c r="S1040" s="2">
+        <v>650</v>
+      </c>
+      <c r="U1040" s="2">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1041">
+        <v>37</v>
+      </c>
+      <c r="C1041" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1041" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1041" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1041" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1041" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1041" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1041">
+        <v>5</v>
+      </c>
+      <c r="N1041">
+        <v>1083</v>
+      </c>
+      <c r="O1041" s="2">
+        <v>5415</v>
+      </c>
+      <c r="P1041" s="2">
+        <v>5415</v>
+      </c>
+      <c r="S1041" s="2">
+        <v>5415</v>
+      </c>
+      <c r="U1041" s="2">
+        <v>5415</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1042">
+        <v>37</v>
+      </c>
+      <c r="C1042" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1042" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1042" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1042" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1042">
+        <v>1.17</v>
+      </c>
+      <c r="H1042">
+        <v>700</v>
+      </c>
+      <c r="I1042" s="2">
+        <v>819</v>
+      </c>
+      <c r="L1042" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1042" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1042" s="2">
+        <v>819</v>
+      </c>
+      <c r="S1042" s="2">
+        <v>819</v>
+      </c>
+      <c r="U1042" s="2">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1043">
+        <v>37</v>
+      </c>
+      <c r="C1043" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1043" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1043" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1043" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1043">
+        <v>3.9</v>
+      </c>
+      <c r="H1043">
+        <v>300</v>
+      </c>
+      <c r="I1043" s="2">
+        <v>1170</v>
+      </c>
+      <c r="L1043" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1043" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1043" s="2">
+        <v>1170</v>
+      </c>
+      <c r="Q1043" s="2">
+        <v>200</v>
+      </c>
+      <c r="S1043" s="2">
+        <v>1370</v>
+      </c>
+      <c r="U1043" s="2">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1044">
+        <v>37</v>
+      </c>
+      <c r="C1044" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1044" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1044" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1044" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1044">
+        <v>3.23</v>
+      </c>
+      <c r="H1044">
+        <v>700</v>
+      </c>
+      <c r="I1044" s="2">
+        <v>2261</v>
+      </c>
+      <c r="J1044">
+        <v>1</v>
+      </c>
+      <c r="K1044">
+        <v>300</v>
+      </c>
+      <c r="L1044" s="2">
+        <v>300</v>
+      </c>
+      <c r="O1044" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1044" s="2">
+        <v>2561</v>
+      </c>
+      <c r="S1044" s="2">
+        <v>2561</v>
+      </c>
+      <c r="U1044" s="2">
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1045">
+        <v>37</v>
+      </c>
+      <c r="C1045" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1045" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1045" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1045" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1045">
+        <v>2.4</v>
+      </c>
+      <c r="H1045">
+        <v>700</v>
+      </c>
+      <c r="I1045" s="2">
+        <v>1680</v>
+      </c>
+      <c r="J1045">
+        <v>1</v>
+      </c>
+      <c r="K1045">
+        <v>300</v>
+      </c>
+      <c r="L1045" s="2">
+        <v>300</v>
+      </c>
+      <c r="O1045" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1045" s="2">
+        <v>1980</v>
+      </c>
+      <c r="S1045" s="2">
+        <v>1980</v>
+      </c>
+      <c r="U1045" s="2">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1046">
+        <v>37</v>
+      </c>
+      <c r="C1046" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1046" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1046" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1046" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1046">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="H1046">
+        <v>700</v>
+      </c>
+      <c r="I1046" s="2">
+        <v>619.5</v>
+      </c>
+      <c r="L1046" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1046" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1046" s="2">
+        <v>619.5</v>
+      </c>
+      <c r="S1046" s="2">
+        <v>619.5</v>
+      </c>
+      <c r="U1046" s="2">
+        <v>619.5</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1047">
+        <v>37</v>
+      </c>
+      <c r="C1047" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1047" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1047" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1047" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1047">
+        <v>0.51</v>
+      </c>
+      <c r="H1047">
+        <v>700</v>
+      </c>
+      <c r="I1047" s="2">
+        <v>357</v>
+      </c>
+      <c r="L1047" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1047" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1047" s="2">
+        <v>357</v>
+      </c>
+      <c r="Q1047" s="2">
+        <v>200</v>
+      </c>
+      <c r="S1047" s="2">
+        <v>557</v>
+      </c>
+      <c r="U1047" s="2">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1048">
+        <v>37</v>
+      </c>
+      <c r="C1048" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1048" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1048" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1048" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1048" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1048">
+        <v>1</v>
+      </c>
+      <c r="K1048">
+        <v>500</v>
+      </c>
+      <c r="L1048" s="2">
+        <v>500</v>
+      </c>
+      <c r="O1048" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1048" s="2">
+        <v>500</v>
+      </c>
+      <c r="S1048" s="2">
+        <v>500</v>
+      </c>
+      <c r="U1048" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1049">
+        <v>37</v>
+      </c>
+      <c r="C1049" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1049" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1049" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1049" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1049" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1049">
+        <v>1</v>
+      </c>
+      <c r="K1049">
+        <v>250</v>
+      </c>
+      <c r="L1049" s="2">
+        <v>250</v>
+      </c>
+      <c r="O1049" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1049" s="2">
+        <v>250</v>
+      </c>
+      <c r="S1049" s="2">
+        <v>250</v>
+      </c>
+      <c r="U1049" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1050">
+        <v>37</v>
+      </c>
+      <c r="C1050" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1050" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1050" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1050" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1050" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1050">
+        <v>1</v>
+      </c>
+      <c r="K1050">
+        <v>250</v>
+      </c>
+      <c r="L1050" s="2">
+        <v>250</v>
+      </c>
+      <c r="O1050" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1050" s="2">
+        <v>250</v>
+      </c>
+      <c r="S1050" s="2">
+        <v>250</v>
+      </c>
+      <c r="U1050" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1051">
+        <v>37</v>
+      </c>
+      <c r="C1051" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1051" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1051" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1051" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1051" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1051">
+        <v>1</v>
+      </c>
+      <c r="K1051">
+        <v>200</v>
+      </c>
+      <c r="L1051" s="2">
+        <v>200</v>
+      </c>
+      <c r="O1051" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1051" s="2">
+        <v>200</v>
+      </c>
+      <c r="S1051" s="2">
+        <v>200</v>
+      </c>
+      <c r="U1051" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1052">
+        <v>37</v>
+      </c>
+      <c r="C1052" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1052" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1052" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1052" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1052" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1052">
+        <v>1</v>
+      </c>
+      <c r="K1052">
+        <v>200</v>
+      </c>
+      <c r="L1052" s="2">
+        <v>200</v>
+      </c>
+      <c r="O1052" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1052" s="2">
+        <v>200</v>
+      </c>
+      <c r="S1052" s="2">
+        <v>200</v>
+      </c>
+      <c r="U1052" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1053">
+        <v>37</v>
+      </c>
+      <c r="C1053" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1053" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1053" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1053" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1053" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1053">
+        <v>1</v>
+      </c>
+      <c r="K1053">
+        <v>500</v>
+      </c>
+      <c r="L1053" s="2">
+        <v>500</v>
+      </c>
+      <c r="O1053" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1053" s="2">
+        <v>500</v>
+      </c>
+      <c r="S1053" s="2">
+        <v>500</v>
+      </c>
+      <c r="U1053" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1054">
+        <v>37</v>
+      </c>
+      <c r="C1054" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1054" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1054" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1054" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1054" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1054">
+        <v>1</v>
+      </c>
+      <c r="K1054">
+        <v>850</v>
+      </c>
+      <c r="L1054" s="2">
+        <v>850</v>
+      </c>
+      <c r="O1054" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1054" s="2">
+        <v>850</v>
+      </c>
+      <c r="S1054" s="2">
+        <v>850</v>
+      </c>
+      <c r="U1054" s="2">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1055">
+        <v>37</v>
+      </c>
+      <c r="C1055" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1055" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1055" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1055" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1055">
+        <v>3.03</v>
+      </c>
+      <c r="H1055">
+        <v>700</v>
+      </c>
+      <c r="I1055" s="2">
+        <v>2121</v>
+      </c>
+      <c r="J1055">
+        <v>1</v>
+      </c>
+      <c r="K1055">
+        <v>250</v>
+      </c>
+      <c r="L1055" s="2">
+        <v>250</v>
+      </c>
+      <c r="O1055" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1055" s="2">
+        <v>2371</v>
+      </c>
+      <c r="S1055" s="2">
+        <v>2371</v>
+      </c>
+      <c r="U1055" s="2">
+        <v>2371</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1056">
+        <v>37</v>
+      </c>
+      <c r="C1056" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1056" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1056" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1056" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1056">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="H1056">
+        <v>400</v>
+      </c>
+      <c r="I1056" s="2">
+        <v>811.99999999999989</v>
+      </c>
+      <c r="J1056">
+        <v>1</v>
+      </c>
+      <c r="K1056">
+        <v>250</v>
+      </c>
+      <c r="L1056" s="2">
+        <v>250</v>
+      </c>
+      <c r="O1056" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1056" s="2">
+        <v>1062</v>
+      </c>
+      <c r="S1056" s="2">
+        <v>1062</v>
+      </c>
+      <c r="U1056" s="2">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1057">
+        <v>37</v>
+      </c>
+      <c r="C1057" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1057" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1057" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1057" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1057">
+        <v>7.5</v>
+      </c>
+      <c r="H1057">
+        <v>250</v>
+      </c>
+      <c r="I1057" s="2">
+        <v>1875</v>
+      </c>
+      <c r="J1057">
+        <v>1</v>
+      </c>
+      <c r="K1057">
+        <v>200</v>
+      </c>
+      <c r="L1057" s="2">
+        <v>200</v>
+      </c>
+      <c r="O1057" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1057" s="2">
+        <v>2075</v>
+      </c>
+      <c r="S1057" s="2">
+        <v>2075</v>
+      </c>
+      <c r="U1057" s="2">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1058">
+        <v>37</v>
+      </c>
+      <c r="C1058" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1058" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1058" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1058" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1058">
+        <v>3.71</v>
+      </c>
+      <c r="H1058">
+        <v>700</v>
+      </c>
+      <c r="I1058" s="2">
+        <v>2597</v>
+      </c>
+      <c r="J1058">
+        <v>1</v>
+      </c>
+      <c r="K1058">
+        <v>200</v>
+      </c>
+      <c r="L1058" s="2">
+        <v>200</v>
+      </c>
+      <c r="O1058" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1058" s="2">
+        <v>2797</v>
+      </c>
+      <c r="S1058" s="2">
+        <v>2797</v>
+      </c>
+      <c r="U1058" s="2">
+        <v>2797</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1059">
+        <v>37</v>
+      </c>
+      <c r="C1059" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1059" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1059" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1059" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1059">
+        <v>2.95</v>
+      </c>
+      <c r="H1059">
+        <v>700</v>
+      </c>
+      <c r="I1059" s="2">
+        <v>2065</v>
+      </c>
+      <c r="L1059" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1059" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1059" s="2">
+        <v>2065</v>
+      </c>
+      <c r="S1059" s="2">
+        <v>2065</v>
+      </c>
+      <c r="U1059" s="2">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1060">
+        <v>37</v>
+      </c>
+      <c r="C1060" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1060" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1060" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1060" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1060">
+        <v>2.95</v>
+      </c>
+      <c r="H1060">
+        <v>700</v>
+      </c>
+      <c r="I1060" s="2">
+        <v>2065</v>
+      </c>
+      <c r="L1060" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1060" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1060" s="2">
+        <v>2065</v>
+      </c>
+      <c r="S1060" s="2">
+        <v>2065</v>
+      </c>
+      <c r="U1060" s="2">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1061">
+        <v>37</v>
+      </c>
+      <c r="C1061" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1061" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1061" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1061" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1061">
+        <v>3.4</v>
+      </c>
+      <c r="H1061">
+        <v>250</v>
+      </c>
+      <c r="I1061" s="2">
+        <v>850</v>
+      </c>
+      <c r="L1061" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1061" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1061" s="2">
+        <v>850</v>
+      </c>
+      <c r="S1061" s="2">
+        <v>850</v>
+      </c>
+      <c r="U1061" s="2">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1062">
+        <v>37</v>
+      </c>
+      <c r="C1062" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1062" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1062" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1062" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1062" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1062">
+        <v>1</v>
+      </c>
+      <c r="K1062">
+        <v>200</v>
+      </c>
+      <c r="L1062" s="2">
+        <v>200</v>
+      </c>
+      <c r="M1062">
+        <v>0.5</v>
+      </c>
+      <c r="N1062">
+        <v>1083.33</v>
+      </c>
+      <c r="O1062" s="2">
+        <v>541.66499999999996</v>
+      </c>
+      <c r="P1062" s="2">
+        <v>741.66499999999996</v>
+      </c>
+      <c r="S1062" s="2">
+        <v>741.66499999999996</v>
+      </c>
+      <c r="U1062" s="2">
+        <v>741.66499999999996</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1063">
+        <v>37</v>
+      </c>
+      <c r="C1063" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1063" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1063" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1063" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1063" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1063">
+        <v>1</v>
+      </c>
+      <c r="K1063">
+        <v>500</v>
+      </c>
+      <c r="L1063" s="2">
+        <v>500</v>
+      </c>
+      <c r="O1063" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1063" s="2">
+        <v>500</v>
+      </c>
+      <c r="S1063" s="2">
+        <v>500</v>
+      </c>
+      <c r="U1063" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1064">
+        <v>37</v>
+      </c>
+      <c r="C1064" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1064" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1064" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1064" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1064" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1064">
+        <v>1</v>
+      </c>
+      <c r="K1064">
+        <v>200</v>
+      </c>
+      <c r="L1064" s="2">
+        <v>200</v>
+      </c>
+      <c r="O1064" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1064" s="2">
+        <v>200</v>
+      </c>
+      <c r="Q1064" s="2">
+        <v>500</v>
+      </c>
+      <c r="S1064" s="2">
+        <v>700</v>
+      </c>
+      <c r="U1064" s="2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1065">
+        <v>37</v>
+      </c>
+      <c r="C1065" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1065" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1065" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1065" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1065">
+        <v>3.2559999999999998</v>
+      </c>
+      <c r="H1065">
+        <v>900</v>
+      </c>
+      <c r="I1065" s="2">
+        <v>2930.3999999999996</v>
+      </c>
+      <c r="L1065" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1065" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1065" s="2">
+        <v>2930.3999999999996</v>
+      </c>
+      <c r="S1065" s="2">
+        <v>2930.3999999999996</v>
+      </c>
+      <c r="U1065" s="2">
+        <v>2930.3999999999996</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1066">
+        <v>37</v>
+      </c>
+      <c r="C1066" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1066" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1066" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1066" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1066">
+        <v>2.544</v>
+      </c>
+      <c r="H1066">
+        <v>400</v>
+      </c>
+      <c r="I1066" s="2">
+        <v>1017.6</v>
+      </c>
+      <c r="L1066" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1066" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1066" s="2">
+        <v>1017.6</v>
+      </c>
+      <c r="Q1066" s="2">
+        <v>300</v>
+      </c>
+      <c r="S1066" s="2">
+        <v>1317.6</v>
+      </c>
+      <c r="U1066" s="2">
+        <v>1317.6</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1067">
+        <v>37</v>
+      </c>
+      <c r="C1067" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1067" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1067" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1067" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1067" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1067" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1067">
+        <v>0.75</v>
+      </c>
+      <c r="N1067">
+        <v>1083.33</v>
+      </c>
+      <c r="O1067" s="2">
+        <v>812.49749999999995</v>
+      </c>
+      <c r="P1067" s="2">
+        <v>812.49749999999995</v>
+      </c>
+      <c r="Q1067" s="2">
+        <v>100</v>
+      </c>
+      <c r="S1067" s="2">
+        <v>912.49749999999995</v>
+      </c>
+      <c r="U1067" s="2">
+        <v>912.49749999999995</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1068">
+        <v>37</v>
+      </c>
+      <c r="C1068" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1068" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1068" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1068" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1068" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1068" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1068">
+        <v>0.75</v>
+      </c>
+      <c r="N1068">
+        <v>1083.33</v>
+      </c>
+      <c r="O1068" s="2">
+        <v>812.49749999999995</v>
+      </c>
+      <c r="P1068" s="2">
+        <v>812.49749999999995</v>
+      </c>
+      <c r="Q1068" s="2">
+        <v>100</v>
+      </c>
+      <c r="S1068" s="2">
+        <v>912.49749999999995</v>
+      </c>
+      <c r="U1068" s="2">
+        <v>912.49749999999995</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1069">
+        <v>37</v>
+      </c>
+      <c r="C1069" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1069" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1069" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1069" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1069">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H1069">
+        <v>700</v>
+      </c>
+      <c r="I1069" s="2">
+        <v>516.6</v>
+      </c>
+      <c r="J1069">
+        <v>1</v>
+      </c>
+      <c r="K1069">
+        <v>200</v>
+      </c>
+      <c r="L1069" s="2">
+        <v>200</v>
+      </c>
+      <c r="M1069">
+        <v>0.25</v>
+      </c>
+      <c r="N1069">
+        <v>750</v>
+      </c>
+      <c r="O1069" s="2">
+        <v>187.5</v>
+      </c>
+      <c r="P1069" s="2">
+        <v>904.1</v>
+      </c>
+      <c r="S1069" s="2">
+        <v>904.1</v>
+      </c>
+      <c r="U1069" s="2">
+        <v>904.1</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1070">
+        <v>37</v>
+      </c>
+      <c r="C1070" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1070" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1070" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1070" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1070">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="H1070">
+        <v>700</v>
+      </c>
+      <c r="I1070" s="2">
+        <v>692.3</v>
+      </c>
+      <c r="J1070">
+        <v>1</v>
+      </c>
+      <c r="K1070">
+        <v>200</v>
+      </c>
+      <c r="L1070" s="2">
+        <v>200</v>
+      </c>
+      <c r="O1070" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1070" s="2">
+        <v>892.3</v>
+      </c>
+      <c r="S1070" s="2">
+        <v>892.3</v>
+      </c>
+      <c r="U1070" s="2">
+        <v>892.3</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1071">
+        <v>37</v>
+      </c>
+      <c r="C1071" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1071" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1071" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1071" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1071" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1071" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1071">
+        <v>2</v>
+      </c>
+      <c r="N1071">
+        <v>750</v>
+      </c>
+      <c r="O1071" s="2">
+        <v>1500</v>
+      </c>
+      <c r="P1071" s="2">
+        <v>1500</v>
+      </c>
+      <c r="S1071" s="2">
+        <v>1500</v>
+      </c>
+      <c r="U1071" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1072">
+        <v>37</v>
+      </c>
+      <c r="C1072" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1072" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1072" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1072" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1072">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="H1072">
+        <v>320</v>
+      </c>
+      <c r="I1072" s="2">
+        <v>716.80000000000007</v>
+      </c>
+      <c r="L1072" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1072">
+        <v>1</v>
+      </c>
+      <c r="N1072">
+        <v>750</v>
+      </c>
+      <c r="O1072" s="2">
+        <v>750</v>
+      </c>
+      <c r="P1072" s="2">
+        <v>1466.8000000000002</v>
+      </c>
+      <c r="S1072" s="2">
+        <v>1466.8000000000002</v>
+      </c>
+      <c r="U1072" s="2">
+        <v>1466.8000000000002</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1073">
+        <v>37</v>
+      </c>
+      <c r="C1073" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1073" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1073" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1073" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1073">
+        <v>1.27</v>
+      </c>
+      <c r="H1073">
+        <v>450</v>
+      </c>
+      <c r="I1073" s="2">
+        <v>571.5</v>
+      </c>
+      <c r="J1073">
+        <v>1</v>
+      </c>
+      <c r="K1073">
+        <v>100</v>
+      </c>
+      <c r="L1073" s="2">
+        <v>100</v>
+      </c>
+      <c r="M1073">
+        <v>1</v>
+      </c>
+      <c r="N1073">
+        <v>1083.33</v>
+      </c>
+      <c r="O1073" s="2">
+        <v>1083.33</v>
+      </c>
+      <c r="P1073" s="2">
+        <v>1754.83</v>
+      </c>
+      <c r="S1073" s="2">
+        <v>1754.83</v>
+      </c>
+      <c r="U1073" s="2">
+        <v>1754.83</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1074">
+        <v>37</v>
+      </c>
+      <c r="C1074" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1074" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1074" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1074" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1074">
+        <v>2.6</v>
+      </c>
+      <c r="H1074">
+        <v>400</v>
+      </c>
+      <c r="I1074" s="2">
+        <v>1040</v>
+      </c>
+      <c r="J1074">
+        <v>1</v>
+      </c>
+      <c r="K1074">
+        <v>850</v>
+      </c>
+      <c r="L1074" s="2">
+        <v>850</v>
+      </c>
+      <c r="O1074" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1074" s="2">
+        <v>1890</v>
+      </c>
+      <c r="S1074" s="2">
+        <v>1890</v>
+      </c>
+      <c r="U1074" s="2">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1075">
+        <v>37</v>
+      </c>
+      <c r="C1075" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1075" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1075" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1075" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1075">
+        <v>3.88</v>
+      </c>
+      <c r="H1075">
+        <v>320</v>
+      </c>
+      <c r="I1075" s="2">
+        <v>1241.5999999999999</v>
+      </c>
+      <c r="L1075" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1075" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1075" s="2">
+        <v>1241.5999999999999</v>
+      </c>
+      <c r="Q1075" s="2">
+        <v>300</v>
+      </c>
+      <c r="S1075" s="2">
+        <v>1541.6</v>
+      </c>
+      <c r="U1075" s="2">
+        <v>1541.6</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1076">
+        <v>37</v>
+      </c>
+      <c r="C1076" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1076" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1076" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1076" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1076" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1076" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1076">
+        <v>2</v>
+      </c>
+      <c r="N1076">
+        <v>750</v>
+      </c>
+      <c r="O1076" s="2">
+        <v>1500</v>
+      </c>
+      <c r="P1076" s="2">
+        <v>1500</v>
+      </c>
+      <c r="Q1076" s="2">
+        <v>400</v>
+      </c>
+      <c r="S1076" s="2">
+        <v>1900</v>
+      </c>
+      <c r="U1076" s="2">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1077">
+        <v>37</v>
+      </c>
+      <c r="C1077" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1077" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1077" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1077" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1077" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1077" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1077">
+        <v>2.5</v>
+      </c>
+      <c r="N1077">
+        <v>750</v>
+      </c>
+      <c r="O1077" s="2">
+        <v>1875</v>
+      </c>
+      <c r="P1077" s="2">
+        <v>1875</v>
+      </c>
+      <c r="S1077" s="2">
+        <v>1875</v>
+      </c>
+      <c r="U1077" s="2">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1078">
+        <v>37</v>
+      </c>
+      <c r="C1078" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1078" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1078" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1078" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1078" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1078" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1078">
+        <v>0.5</v>
+      </c>
+      <c r="N1078">
+        <v>750</v>
+      </c>
+      <c r="O1078" s="2">
+        <v>375</v>
+      </c>
+      <c r="P1078" s="2">
+        <v>375</v>
+      </c>
+      <c r="S1078" s="2">
+        <v>375</v>
+      </c>
+      <c r="U1078" s="2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1079">
+        <v>37</v>
+      </c>
+      <c r="C1079" s="1">
+        <v>45548</v>
+      </c>
+      <c r="D1079" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1079" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1079" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1079" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1079" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1079">
+        <v>1.25</v>
+      </c>
+      <c r="N1079">
+        <v>750</v>
+      </c>
+      <c r="O1079" s="2">
+        <v>937.5</v>
+      </c>
+      <c r="P1079" s="2">
+        <v>937.5</v>
+      </c>
+      <c r="S1079" s="2">
+        <v>937.5</v>
+      </c>
+      <c r="U1079" s="2">
+        <v>937.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Destajo Hrs Prod Sem 38
</commit_message>
<xml_diff>
--- a/datasets/destajo.xlsx
+++ b/datasets/destajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/275e1cc0366b6475/Documentos/Vori Vost/Pruebas-Boton/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{48AB0E75-7D41-47DC-B758-D10181A064D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67FCFB52-4134-40DE-97AC-0B36385E13F5}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{48AB0E75-7D41-47DC-B758-D10181A064D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77968C0C-06E9-4BC6-9389-59168370758C}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{31EFA5F5-4BB3-40E1-95BE-59439A9739F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3256" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3373" uniqueCount="142">
   <si>
     <t>SEMANA</t>
   </si>
@@ -439,6 +439,30 @@
   <si>
     <t>CTVV 1176 - CASA ANDREA SANCHEZ - ANDREA SANCHEZ</t>
   </si>
+  <si>
+    <t>CTVV 3142</t>
+  </si>
+  <si>
+    <t>CTVV 3142 - Propuesta Verona Zamora (10 casas) - Meda</t>
+  </si>
+  <si>
+    <t>CTVV 3161</t>
+  </si>
+  <si>
+    <t>CTVV 3161 - Reemplazo de Mobiliario - Hogares Deesa</t>
+  </si>
+  <si>
+    <t>CTVV 3073</t>
+  </si>
+  <si>
+    <t>CTVV 3073 - Librero Niño - Cristina Barba</t>
+  </si>
+  <si>
+    <t>CTVV 2319</t>
+  </si>
+  <si>
+    <t>CTVV 2319 - COCINA ALEJANDRO RUIZ</t>
+  </si>
 </sst>
 </file>
 
@@ -510,13 +534,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}" name="Tabla3" displayName="Tabla3" ref="A1:V1079" totalsRowShown="0">
-  <autoFilter ref="A1:V1079" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}" name="Tabla3" displayName="Tabla3" ref="A1:V1118" totalsRowShown="0">
+  <autoFilter ref="A1:V1118" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}"/>
   <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{50CD881F-F4BE-4F9A-B2C3-50C2D8C2910F}" name="SEMANA"/>
     <tableColumn id="2" xr3:uid="{54EA7CC6-3702-4F53-8DD3-E9431860F33D}" name="PERÍODO"/>
@@ -862,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD62827-3B7E-49B3-B2B1-64E636F38ACC}">
-  <dimension ref="A1:V1079"/>
+  <dimension ref="A1:V1118"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1057" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1069" sqref="F1069"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1104" sqref="F1104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -48269,6 +48289,1662 @@
         <v>937.5</v>
       </c>
     </row>
+    <row r="1080" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1080">
+        <v>38</v>
+      </c>
+      <c r="C1080" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1080" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1080" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1080" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1080">
+        <v>1.85</v>
+      </c>
+      <c r="H1080">
+        <v>700</v>
+      </c>
+      <c r="I1080" s="2">
+        <v>1295</v>
+      </c>
+      <c r="L1080" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1080" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1080" s="2">
+        <v>1295</v>
+      </c>
+      <c r="S1080" s="2">
+        <v>1295</v>
+      </c>
+      <c r="U1080" s="2">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1081">
+        <v>38</v>
+      </c>
+      <c r="C1081" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1081" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1081" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1081" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1081">
+        <v>1.57</v>
+      </c>
+      <c r="H1081">
+        <v>700</v>
+      </c>
+      <c r="I1081" s="2">
+        <v>1099</v>
+      </c>
+      <c r="L1081" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1081" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1081" s="2">
+        <v>1099</v>
+      </c>
+      <c r="S1081" s="2">
+        <v>1099</v>
+      </c>
+      <c r="U1081" s="2">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1082">
+        <v>38</v>
+      </c>
+      <c r="C1082" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1082" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1082" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1082" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1082">
+        <v>1.85</v>
+      </c>
+      <c r="H1082">
+        <v>700</v>
+      </c>
+      <c r="I1082" s="2">
+        <v>1295</v>
+      </c>
+      <c r="L1082" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1082" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1082" s="2">
+        <v>1295</v>
+      </c>
+      <c r="S1082" s="2">
+        <v>1295</v>
+      </c>
+      <c r="U1082" s="2">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1083">
+        <v>38</v>
+      </c>
+      <c r="C1083" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1083" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1083" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1083" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1083">
+        <v>0.73</v>
+      </c>
+      <c r="H1083">
+        <v>700</v>
+      </c>
+      <c r="I1083" s="2">
+        <v>511</v>
+      </c>
+      <c r="L1083" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1083" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1083" s="2">
+        <v>511</v>
+      </c>
+      <c r="S1083" s="2">
+        <v>511</v>
+      </c>
+      <c r="U1083" s="2">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1084">
+        <v>38</v>
+      </c>
+      <c r="C1084" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1084" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1084" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1084" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1084">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="H1084">
+        <v>700</v>
+      </c>
+      <c r="I1084" s="2">
+        <v>619.5</v>
+      </c>
+      <c r="J1084">
+        <v>1</v>
+      </c>
+      <c r="K1084">
+        <v>350</v>
+      </c>
+      <c r="L1084" s="2">
+        <v>350</v>
+      </c>
+      <c r="O1084" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1084" s="2">
+        <v>969.5</v>
+      </c>
+      <c r="S1084" s="2">
+        <v>969.5</v>
+      </c>
+      <c r="U1084" s="2">
+        <v>969.5</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1085">
+        <v>38</v>
+      </c>
+      <c r="C1085" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1085" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1085" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1085" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1085">
+        <v>0.51</v>
+      </c>
+      <c r="H1085">
+        <v>700</v>
+      </c>
+      <c r="I1085" s="2">
+        <v>357</v>
+      </c>
+      <c r="L1085" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1085" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1085" s="2">
+        <v>357</v>
+      </c>
+      <c r="Q1085" s="2">
+        <v>500</v>
+      </c>
+      <c r="S1085" s="2">
+        <v>857</v>
+      </c>
+      <c r="U1085" s="2">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1086">
+        <v>38</v>
+      </c>
+      <c r="C1086" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1086" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1086" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1086" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1086" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1086" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1086">
+        <v>1.25</v>
+      </c>
+      <c r="N1086">
+        <v>750</v>
+      </c>
+      <c r="O1086" s="2">
+        <v>937.5</v>
+      </c>
+      <c r="P1086" s="2">
+        <v>937.5</v>
+      </c>
+      <c r="S1086" s="2">
+        <v>937.5</v>
+      </c>
+      <c r="U1086" s="2">
+        <v>937.5</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1087">
+        <v>38</v>
+      </c>
+      <c r="C1087" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1087" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1087" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1087" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1087" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1087" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1087">
+        <v>5</v>
+      </c>
+      <c r="N1087">
+        <v>1083</v>
+      </c>
+      <c r="O1087" s="2">
+        <v>5415</v>
+      </c>
+      <c r="P1087" s="2">
+        <v>5415</v>
+      </c>
+      <c r="S1087" s="2">
+        <v>5415</v>
+      </c>
+      <c r="U1087" s="2">
+        <v>5415</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1088">
+        <v>38</v>
+      </c>
+      <c r="C1088" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1088" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1088" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1088" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1088">
+        <v>2.8</v>
+      </c>
+      <c r="H1088">
+        <v>700</v>
+      </c>
+      <c r="I1088" s="2">
+        <v>1959.9999999999998</v>
+      </c>
+      <c r="L1088" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1088" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1088" s="2">
+        <v>1959.9999999999998</v>
+      </c>
+      <c r="S1088" s="2">
+        <v>1959.9999999999998</v>
+      </c>
+      <c r="U1088" s="2">
+        <v>1959.9999999999998</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1089">
+        <v>38</v>
+      </c>
+      <c r="C1089" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1089" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1089" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1089" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1089">
+        <v>1.35</v>
+      </c>
+      <c r="H1089">
+        <v>400</v>
+      </c>
+      <c r="I1089" s="2">
+        <v>540</v>
+      </c>
+      <c r="J1089">
+        <v>1</v>
+      </c>
+      <c r="K1089">
+        <v>200</v>
+      </c>
+      <c r="L1089" s="2">
+        <v>200</v>
+      </c>
+      <c r="M1089">
+        <v>0.5</v>
+      </c>
+      <c r="N1089">
+        <v>750</v>
+      </c>
+      <c r="O1089" s="2">
+        <v>375</v>
+      </c>
+      <c r="P1089" s="2">
+        <v>1115</v>
+      </c>
+      <c r="S1089" s="2">
+        <v>1115</v>
+      </c>
+      <c r="U1089" s="2">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1090">
+        <v>38</v>
+      </c>
+      <c r="C1090" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1090" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1090" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1090" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1090">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H1090">
+        <v>700</v>
+      </c>
+      <c r="I1090" s="2">
+        <v>406</v>
+      </c>
+      <c r="L1090" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1090" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1090" s="2">
+        <v>406</v>
+      </c>
+      <c r="S1090" s="2">
+        <v>406</v>
+      </c>
+      <c r="U1090" s="2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1091">
+        <v>38</v>
+      </c>
+      <c r="C1091" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1091" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1091" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1091" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1091">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="H1091">
+        <v>700</v>
+      </c>
+      <c r="I1091" s="2">
+        <v>632.1</v>
+      </c>
+      <c r="L1091" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1091">
+        <v>1.5</v>
+      </c>
+      <c r="N1091">
+        <v>1083.33</v>
+      </c>
+      <c r="O1091" s="2">
+        <v>1624.9949999999999</v>
+      </c>
+      <c r="P1091" s="2">
+        <v>2257.0949999999998</v>
+      </c>
+      <c r="S1091" s="2">
+        <v>2257.0949999999998</v>
+      </c>
+      <c r="U1091" s="2">
+        <v>2257.0949999999998</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1092">
+        <v>38</v>
+      </c>
+      <c r="C1092" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1092" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1092" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1092" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1092">
+        <v>3.63</v>
+      </c>
+      <c r="H1092">
+        <v>800</v>
+      </c>
+      <c r="I1092" s="2">
+        <v>2904</v>
+      </c>
+      <c r="J1092">
+        <v>1</v>
+      </c>
+      <c r="K1092">
+        <v>200</v>
+      </c>
+      <c r="L1092" s="2">
+        <v>200</v>
+      </c>
+      <c r="O1092" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1092" s="2">
+        <v>3104</v>
+      </c>
+      <c r="S1092" s="2">
+        <v>3104</v>
+      </c>
+      <c r="U1092" s="2">
+        <v>3104</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1093">
+        <v>38</v>
+      </c>
+      <c r="C1093" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1093" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1093" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1093" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1093">
+        <v>0.8</v>
+      </c>
+      <c r="H1093">
+        <v>500</v>
+      </c>
+      <c r="I1093" s="2">
+        <v>400</v>
+      </c>
+      <c r="L1093" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1093" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1093" s="2">
+        <v>400</v>
+      </c>
+      <c r="S1093" s="2">
+        <v>400</v>
+      </c>
+      <c r="U1093" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1094">
+        <v>38</v>
+      </c>
+      <c r="C1094" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1094" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1094" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1094" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1094">
+        <v>1.81</v>
+      </c>
+      <c r="H1094">
+        <v>350</v>
+      </c>
+      <c r="I1094" s="2">
+        <v>633.5</v>
+      </c>
+      <c r="L1094" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1094" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1094" s="2">
+        <v>633.5</v>
+      </c>
+      <c r="S1094" s="2">
+        <v>633.5</v>
+      </c>
+      <c r="U1094" s="2">
+        <v>633.5</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1095">
+        <v>38</v>
+      </c>
+      <c r="C1095" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1095" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1095" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1095" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1095">
+        <v>2.12</v>
+      </c>
+      <c r="H1095">
+        <v>170</v>
+      </c>
+      <c r="I1095" s="2">
+        <v>360.40000000000003</v>
+      </c>
+      <c r="L1095" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1095" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1095" s="2">
+        <v>360.40000000000003</v>
+      </c>
+      <c r="S1095" s="2">
+        <v>360.40000000000003</v>
+      </c>
+      <c r="U1095" s="2">
+        <v>360.40000000000003</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1096">
+        <v>38</v>
+      </c>
+      <c r="C1096" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1096" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1096" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1096" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1096" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1096">
+        <v>1</v>
+      </c>
+      <c r="K1096">
+        <v>1800</v>
+      </c>
+      <c r="L1096" s="2">
+        <v>1800</v>
+      </c>
+      <c r="O1096" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1096" s="2">
+        <v>1800</v>
+      </c>
+      <c r="S1096" s="2">
+        <v>1800</v>
+      </c>
+      <c r="U1096" s="2">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1097">
+        <v>38</v>
+      </c>
+      <c r="C1097" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1097" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1097" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1097" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1097">
+        <v>3.0150000000000001</v>
+      </c>
+      <c r="H1097">
+        <v>250</v>
+      </c>
+      <c r="I1097" s="2">
+        <v>753.75</v>
+      </c>
+      <c r="L1097" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1097" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1097" s="2">
+        <v>753.75</v>
+      </c>
+      <c r="S1097" s="2">
+        <v>753.75</v>
+      </c>
+      <c r="U1097" s="2">
+        <v>753.75</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1098">
+        <v>38</v>
+      </c>
+      <c r="C1098" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1098" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1098" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1098" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1098" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1098">
+        <v>6</v>
+      </c>
+      <c r="K1098">
+        <v>700</v>
+      </c>
+      <c r="L1098" s="2">
+        <v>4200</v>
+      </c>
+      <c r="O1098" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1098" s="2">
+        <v>4200</v>
+      </c>
+      <c r="S1098" s="2">
+        <v>4200</v>
+      </c>
+      <c r="U1098" s="2">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1099">
+        <v>38</v>
+      </c>
+      <c r="C1099" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1099" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1099" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1099" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1099" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1099">
+        <v>2</v>
+      </c>
+      <c r="K1099">
+        <v>750</v>
+      </c>
+      <c r="L1099" s="2">
+        <v>1500</v>
+      </c>
+      <c r="O1099" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1099" s="2">
+        <v>1500</v>
+      </c>
+      <c r="S1099" s="2">
+        <v>1500</v>
+      </c>
+      <c r="U1099" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1100">
+        <v>38</v>
+      </c>
+      <c r="C1100" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1100" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1100" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1100" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1100" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1100">
+        <v>1</v>
+      </c>
+      <c r="K1100">
+        <v>500</v>
+      </c>
+      <c r="L1100" s="2">
+        <v>500</v>
+      </c>
+      <c r="O1100" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1100" s="2">
+        <v>500</v>
+      </c>
+      <c r="Q1100" s="2">
+        <v>500</v>
+      </c>
+      <c r="S1100" s="2">
+        <v>1000</v>
+      </c>
+      <c r="U1100" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1101">
+        <v>38</v>
+      </c>
+      <c r="C1101" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1101" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1101" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1101" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1101">
+        <v>0.98</v>
+      </c>
+      <c r="H1101">
+        <v>600</v>
+      </c>
+      <c r="I1101" s="2">
+        <v>588</v>
+      </c>
+      <c r="L1101" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1101" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1101" s="2">
+        <v>588</v>
+      </c>
+      <c r="S1101" s="2">
+        <v>588</v>
+      </c>
+      <c r="U1101" s="2">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1102">
+        <v>38</v>
+      </c>
+      <c r="C1102" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1102" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1102" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1102" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1102">
+        <v>3.18</v>
+      </c>
+      <c r="H1102">
+        <v>250</v>
+      </c>
+      <c r="I1102" s="2">
+        <v>795</v>
+      </c>
+      <c r="L1102" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1102" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1102" s="2">
+        <v>795</v>
+      </c>
+      <c r="S1102" s="2">
+        <v>795</v>
+      </c>
+      <c r="U1102" s="2">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1103">
+        <v>38</v>
+      </c>
+      <c r="C1103" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1103" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1103" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1103" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1103">
+        <v>5.53</v>
+      </c>
+      <c r="H1103">
+        <v>300</v>
+      </c>
+      <c r="I1103" s="2">
+        <v>1659</v>
+      </c>
+      <c r="L1103" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1103" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1103" s="2">
+        <v>1659</v>
+      </c>
+      <c r="S1103" s="2">
+        <v>1659</v>
+      </c>
+      <c r="U1103" s="2">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1104">
+        <v>38</v>
+      </c>
+      <c r="C1104" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1104" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1104" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1104" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1104" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1104" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1104">
+        <v>1</v>
+      </c>
+      <c r="N1104">
+        <v>750</v>
+      </c>
+      <c r="O1104" s="2">
+        <v>750</v>
+      </c>
+      <c r="P1104" s="2">
+        <v>750</v>
+      </c>
+      <c r="S1104" s="2">
+        <v>750</v>
+      </c>
+      <c r="U1104" s="2">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1105">
+        <v>38</v>
+      </c>
+      <c r="C1105" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1105" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1105" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1105" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1105" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1105" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1105">
+        <v>1</v>
+      </c>
+      <c r="N1105">
+        <v>750</v>
+      </c>
+      <c r="O1105" s="2">
+        <v>750</v>
+      </c>
+      <c r="P1105" s="2">
+        <v>750</v>
+      </c>
+      <c r="S1105" s="2">
+        <v>750</v>
+      </c>
+      <c r="U1105" s="2">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1106">
+        <v>38</v>
+      </c>
+      <c r="C1106" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1106" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1106" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1106" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1106" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1106">
+        <v>4</v>
+      </c>
+      <c r="N1106">
+        <v>700</v>
+      </c>
+      <c r="O1106" s="2">
+        <v>2800</v>
+      </c>
+      <c r="P1106" s="2">
+        <v>2800</v>
+      </c>
+      <c r="Q1106" s="2">
+        <v>400</v>
+      </c>
+      <c r="S1106" s="2">
+        <v>3200</v>
+      </c>
+      <c r="U1106" s="2">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1107">
+        <v>38</v>
+      </c>
+      <c r="C1107" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1107" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1107" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1107" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1107" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1107">
+        <v>1</v>
+      </c>
+      <c r="K1107">
+        <v>700</v>
+      </c>
+      <c r="L1107" s="2">
+        <v>700</v>
+      </c>
+      <c r="O1107" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1107" s="2">
+        <v>700</v>
+      </c>
+      <c r="S1107" s="2">
+        <v>700</v>
+      </c>
+      <c r="U1107" s="2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1108">
+        <v>38</v>
+      </c>
+      <c r="C1108" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1108" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1108" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1108" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1108" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1108" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1108">
+        <v>0.5</v>
+      </c>
+      <c r="N1108">
+        <v>1083.33</v>
+      </c>
+      <c r="O1108" s="2">
+        <v>541.66499999999996</v>
+      </c>
+      <c r="P1108" s="2">
+        <v>541.66499999999996</v>
+      </c>
+      <c r="Q1108" s="2">
+        <v>100</v>
+      </c>
+      <c r="S1108" s="2">
+        <v>641.66499999999996</v>
+      </c>
+      <c r="U1108" s="2">
+        <v>641.66499999999996</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1109">
+        <v>38</v>
+      </c>
+      <c r="C1109" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1109" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1109" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1109" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1109" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1109">
+        <v>3</v>
+      </c>
+      <c r="K1109">
+        <v>850</v>
+      </c>
+      <c r="L1109" s="2">
+        <v>2550</v>
+      </c>
+      <c r="M1109">
+        <v>0.5</v>
+      </c>
+      <c r="N1109">
+        <v>1083.33</v>
+      </c>
+      <c r="O1109" s="2">
+        <v>541.66499999999996</v>
+      </c>
+      <c r="P1109" s="2">
+        <v>3091.665</v>
+      </c>
+      <c r="S1109" s="2">
+        <v>3091.665</v>
+      </c>
+      <c r="U1109" s="2">
+        <v>3091.665</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1110">
+        <v>38</v>
+      </c>
+      <c r="C1110" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1110" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1110" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1110" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1110" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1110">
+        <v>1</v>
+      </c>
+      <c r="K1110">
+        <v>700</v>
+      </c>
+      <c r="L1110" s="2">
+        <v>700</v>
+      </c>
+      <c r="O1110" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1110" s="2">
+        <v>700</v>
+      </c>
+      <c r="S1110" s="2">
+        <v>700</v>
+      </c>
+      <c r="U1110" s="2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1111">
+        <v>38</v>
+      </c>
+      <c r="C1111" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1111" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1111" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1111" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1111" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1111" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1111">
+        <v>1</v>
+      </c>
+      <c r="N1111">
+        <v>1083.33</v>
+      </c>
+      <c r="O1111" s="2">
+        <v>1083.33</v>
+      </c>
+      <c r="P1111" s="2">
+        <v>1083.33</v>
+      </c>
+      <c r="Q1111" s="2">
+        <v>100</v>
+      </c>
+      <c r="S1111" s="2">
+        <v>1183.33</v>
+      </c>
+      <c r="U1111" s="2">
+        <v>1183.33</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1112">
+        <v>38</v>
+      </c>
+      <c r="C1112" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1112" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1112" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1112" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1112" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1112" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1112">
+        <v>0.75</v>
+      </c>
+      <c r="N1112">
+        <v>1083.33</v>
+      </c>
+      <c r="O1112" s="2">
+        <v>812.49749999999995</v>
+      </c>
+      <c r="P1112" s="2">
+        <v>812.49749999999995</v>
+      </c>
+      <c r="S1112" s="2">
+        <v>812.49749999999995</v>
+      </c>
+      <c r="U1112" s="2">
+        <v>812.49749999999995</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1113">
+        <v>38</v>
+      </c>
+      <c r="C1113" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1113" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1113" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1113" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1113" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1113" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1113">
+        <v>0.125</v>
+      </c>
+      <c r="N1113">
+        <v>750</v>
+      </c>
+      <c r="O1113" s="2">
+        <v>93.75</v>
+      </c>
+      <c r="P1113" s="2">
+        <v>93.75</v>
+      </c>
+      <c r="S1113" s="2">
+        <v>93.75</v>
+      </c>
+      <c r="U1113" s="2">
+        <v>93.75</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1114">
+        <v>38</v>
+      </c>
+      <c r="C1114" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1114" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1114" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1114" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1114" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1114" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1114">
+        <v>1</v>
+      </c>
+      <c r="N1114">
+        <v>750</v>
+      </c>
+      <c r="O1114" s="2">
+        <v>750</v>
+      </c>
+      <c r="P1114" s="2">
+        <v>750</v>
+      </c>
+      <c r="S1114" s="2">
+        <v>750</v>
+      </c>
+      <c r="U1114" s="2">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1115">
+        <v>38</v>
+      </c>
+      <c r="C1115" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1115" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1115" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1115" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1115">
+        <v>1.17</v>
+      </c>
+      <c r="H1115">
+        <v>700</v>
+      </c>
+      <c r="I1115" s="2">
+        <v>819</v>
+      </c>
+      <c r="J1115">
+        <v>1</v>
+      </c>
+      <c r="K1115">
+        <v>500</v>
+      </c>
+      <c r="L1115" s="2">
+        <v>500</v>
+      </c>
+      <c r="O1115" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1115" s="2">
+        <v>1319</v>
+      </c>
+      <c r="S1115" s="2">
+        <v>1319</v>
+      </c>
+      <c r="U1115" s="2">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1116">
+        <v>38</v>
+      </c>
+      <c r="C1116" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1116" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1116" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1116" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1116">
+        <v>2.27</v>
+      </c>
+      <c r="H1116">
+        <v>320</v>
+      </c>
+      <c r="I1116" s="2">
+        <v>726.4</v>
+      </c>
+      <c r="L1116" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1116" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1116" s="2">
+        <v>726.4</v>
+      </c>
+      <c r="S1116" s="2">
+        <v>726.4</v>
+      </c>
+      <c r="U1116" s="2">
+        <v>726.4</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1117">
+        <v>38</v>
+      </c>
+      <c r="C1117" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1117" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1117" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1117" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1117">
+        <v>1.65</v>
+      </c>
+      <c r="H1117">
+        <v>700</v>
+      </c>
+      <c r="I1117" s="2">
+        <v>1155</v>
+      </c>
+      <c r="L1117" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1117" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1117" s="2">
+        <v>1155</v>
+      </c>
+      <c r="S1117" s="2">
+        <v>1155</v>
+      </c>
+      <c r="U1117" s="2">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1118">
+        <v>38</v>
+      </c>
+      <c r="C1118" s="1">
+        <v>45555</v>
+      </c>
+      <c r="D1118" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1118" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1118" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1118">
+        <v>0.9</v>
+      </c>
+      <c r="H1118">
+        <v>700</v>
+      </c>
+      <c r="I1118" s="2">
+        <v>630</v>
+      </c>
+      <c r="L1118" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1118" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1118" s="2">
+        <v>630</v>
+      </c>
+      <c r="S1118" s="2">
+        <v>630</v>
+      </c>
+      <c r="U1118" s="2">
+        <v>630</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Destajo Sem 40 sin tablas y totales c/formato
</commit_message>
<xml_diff>
--- a/datasets/destajo.xlsx
+++ b/datasets/destajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/275e1cc0366b6475/Documentos/Vori Vost/Pruebas-Boton/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{48AB0E75-7D41-47DC-B758-D10181A064D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D62FE19D-DB05-4298-9ACB-D1379C8EF799}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{48AB0E75-7D41-47DC-B758-D10181A064D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96E56579-9437-4424-979B-69BF4A39C4F2}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{31EFA5F5-4BB3-40E1-95BE-59439A9739F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3520" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3625" uniqueCount="148">
   <si>
     <t>SEMANA</t>
   </si>
@@ -475,6 +475,12 @@
   <si>
     <t>CTVV 3125 - Remodelación Puerta Sur - Verónica Erón</t>
   </si>
+  <si>
+    <t>CTVV 2109</t>
+  </si>
+  <si>
+    <t>CTVV 2109 - CASA SO MODISA - MODISA</t>
+  </si>
 </sst>
 </file>
 
@@ -547,8 +553,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}" name="Tabla3" displayName="Tabla3" ref="A1:V1167" totalsRowShown="0">
-  <autoFilter ref="A1:V1167" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}" name="Tabla3" displayName="Tabla3" ref="A1:V1202" totalsRowShown="0">
+  <autoFilter ref="A1:V1202" xr:uid="{9E0CC650-65D8-433D-B952-D6D8E7051F24}"/>
   <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{50CD881F-F4BE-4F9A-B2C3-50C2D8C2910F}" name="SEMANA"/>
     <tableColumn id="2" xr3:uid="{54EA7CC6-3702-4F53-8DD3-E9431860F33D}" name="PERÍODO"/>
@@ -894,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD62827-3B7E-49B3-B2B1-64E636F38ACC}">
-  <dimension ref="A1:V1167"/>
+  <dimension ref="A1:V1202"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1102" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1113" sqref="E1113"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1154" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1168" sqref="A1168:V1202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -52092,6 +52098,1519 @@
         <v>1106</v>
       </c>
     </row>
+    <row r="1168" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1168">
+        <v>40</v>
+      </c>
+      <c r="C1168" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1168" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1168" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1168" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1168" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1168" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1168">
+        <v>1</v>
+      </c>
+      <c r="N1168">
+        <v>750</v>
+      </c>
+      <c r="O1168" s="2">
+        <v>750</v>
+      </c>
+      <c r="P1168" s="2">
+        <v>750</v>
+      </c>
+      <c r="S1168" s="2">
+        <v>750</v>
+      </c>
+      <c r="U1168" s="2">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1169">
+        <v>40</v>
+      </c>
+      <c r="C1169" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1169" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1169" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1169" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1169" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1169" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1169">
+        <v>0.5</v>
+      </c>
+      <c r="N1169">
+        <v>700</v>
+      </c>
+      <c r="O1169" s="2">
+        <v>350</v>
+      </c>
+      <c r="P1169" s="2">
+        <v>350</v>
+      </c>
+      <c r="S1169" s="2">
+        <v>350</v>
+      </c>
+      <c r="U1169" s="2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1170">
+        <v>40</v>
+      </c>
+      <c r="C1170" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1170" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1170" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1170" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1170">
+        <v>0.85</v>
+      </c>
+      <c r="H1170">
+        <v>700</v>
+      </c>
+      <c r="I1170" s="2">
+        <v>595</v>
+      </c>
+      <c r="J1170">
+        <v>1</v>
+      </c>
+      <c r="K1170">
+        <v>365</v>
+      </c>
+      <c r="L1170" s="2">
+        <v>365</v>
+      </c>
+      <c r="M1170">
+        <v>1</v>
+      </c>
+      <c r="N1170">
+        <v>750</v>
+      </c>
+      <c r="O1170" s="2">
+        <v>750</v>
+      </c>
+      <c r="P1170" s="2">
+        <v>1710</v>
+      </c>
+      <c r="S1170" s="2">
+        <v>1710</v>
+      </c>
+      <c r="U1170" s="2">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1171">
+        <v>40</v>
+      </c>
+      <c r="C1171" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1171" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1171" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1171" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1171">
+        <v>2.59</v>
+      </c>
+      <c r="H1171">
+        <v>350</v>
+      </c>
+      <c r="I1171" s="2">
+        <v>906.5</v>
+      </c>
+      <c r="J1171">
+        <v>1</v>
+      </c>
+      <c r="K1171">
+        <v>700</v>
+      </c>
+      <c r="L1171" s="2">
+        <v>700</v>
+      </c>
+      <c r="O1171" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1171" s="2">
+        <v>1606.5</v>
+      </c>
+      <c r="S1171" s="2">
+        <v>1606.5</v>
+      </c>
+      <c r="U1171" s="2">
+        <v>1606.5</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1172">
+        <v>40</v>
+      </c>
+      <c r="C1172" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1172" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1172" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1172" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1172">
+        <v>0.71</v>
+      </c>
+      <c r="H1172">
+        <v>700</v>
+      </c>
+      <c r="I1172" s="2">
+        <v>497</v>
+      </c>
+      <c r="L1172" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1172" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1172" s="2">
+        <v>497</v>
+      </c>
+      <c r="Q1172" s="2">
+        <v>500</v>
+      </c>
+      <c r="S1172" s="2">
+        <v>997</v>
+      </c>
+      <c r="U1172" s="2">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1173">
+        <v>40</v>
+      </c>
+      <c r="C1173" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1173" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1173" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1173" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1173">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="H1173">
+        <v>320</v>
+      </c>
+      <c r="I1173" s="2">
+        <v>348.8</v>
+      </c>
+      <c r="J1173">
+        <v>2</v>
+      </c>
+      <c r="K1173">
+        <v>300</v>
+      </c>
+      <c r="L1173" s="2">
+        <v>600</v>
+      </c>
+      <c r="O1173" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1173" s="2">
+        <v>948.8</v>
+      </c>
+      <c r="S1173" s="2">
+        <v>948.8</v>
+      </c>
+      <c r="U1173" s="2">
+        <v>948.8</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1174">
+        <v>40</v>
+      </c>
+      <c r="C1174" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1174" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1174" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1174" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1174">
+        <v>0.81</v>
+      </c>
+      <c r="H1174">
+        <v>700</v>
+      </c>
+      <c r="I1174" s="2">
+        <v>567</v>
+      </c>
+      <c r="J1174">
+        <v>1</v>
+      </c>
+      <c r="K1174">
+        <v>150</v>
+      </c>
+      <c r="L1174" s="2">
+        <v>150</v>
+      </c>
+      <c r="O1174" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1174" s="2">
+        <v>717</v>
+      </c>
+      <c r="S1174" s="2">
+        <v>717</v>
+      </c>
+      <c r="U1174" s="2">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1175">
+        <v>40</v>
+      </c>
+      <c r="C1175" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1175" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1175" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1175" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1175">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="H1175">
+        <v>320</v>
+      </c>
+      <c r="I1175" s="2">
+        <v>348.8</v>
+      </c>
+      <c r="L1175" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1175" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1175" s="2">
+        <v>348.8</v>
+      </c>
+      <c r="S1175" s="2">
+        <v>348.8</v>
+      </c>
+      <c r="U1175" s="2">
+        <v>348.8</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1176">
+        <v>40</v>
+      </c>
+      <c r="C1176" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1176" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1176" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1176" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1176">
+        <v>1.9</v>
+      </c>
+      <c r="H1176">
+        <v>700</v>
+      </c>
+      <c r="I1176" s="2">
+        <v>1330</v>
+      </c>
+      <c r="L1176" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1176" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1176" s="2">
+        <v>1330</v>
+      </c>
+      <c r="S1176" s="2">
+        <v>1330</v>
+      </c>
+      <c r="U1176" s="2">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1177">
+        <v>40</v>
+      </c>
+      <c r="C1177" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1177" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1177" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1177" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1177">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="H1177">
+        <v>320</v>
+      </c>
+      <c r="I1177" s="2">
+        <v>348.8</v>
+      </c>
+      <c r="L1177" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1177" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1177" s="2">
+        <v>348.8</v>
+      </c>
+      <c r="S1177" s="2">
+        <v>348.8</v>
+      </c>
+      <c r="U1177" s="2">
+        <v>348.8</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1178">
+        <v>40</v>
+      </c>
+      <c r="C1178" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1178" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1178" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1178" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1178">
+        <v>1.9</v>
+      </c>
+      <c r="H1178">
+        <v>700</v>
+      </c>
+      <c r="I1178" s="2">
+        <v>1330</v>
+      </c>
+      <c r="L1178" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1178" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1178" s="2">
+        <v>1330</v>
+      </c>
+      <c r="S1178" s="2">
+        <v>1330</v>
+      </c>
+      <c r="U1178" s="2">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1179">
+        <v>40</v>
+      </c>
+      <c r="C1179" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1179" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1179" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1179" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1179">
+        <v>2.27</v>
+      </c>
+      <c r="H1179">
+        <v>320</v>
+      </c>
+      <c r="I1179" s="2">
+        <v>726.4</v>
+      </c>
+      <c r="J1179">
+        <v>1</v>
+      </c>
+      <c r="K1179">
+        <v>500</v>
+      </c>
+      <c r="L1179" s="2">
+        <v>500</v>
+      </c>
+      <c r="O1179" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1179" s="2">
+        <v>1226.4000000000001</v>
+      </c>
+      <c r="S1179" s="2">
+        <v>1226.4000000000001</v>
+      </c>
+      <c r="U1179" s="2">
+        <v>1226.4000000000001</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1180">
+        <v>40</v>
+      </c>
+      <c r="C1180" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1180" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1180" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1180" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1180">
+        <v>2.16</v>
+      </c>
+      <c r="H1180">
+        <v>700</v>
+      </c>
+      <c r="I1180" s="2">
+        <v>1512</v>
+      </c>
+      <c r="L1180" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1180" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1180" s="2">
+        <v>1512</v>
+      </c>
+      <c r="S1180" s="2">
+        <v>1512</v>
+      </c>
+      <c r="U1180" s="2">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1181">
+        <v>40</v>
+      </c>
+      <c r="C1181" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1181" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1181" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1181" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1181">
+        <v>2.8</v>
+      </c>
+      <c r="H1181">
+        <v>700</v>
+      </c>
+      <c r="I1181" s="2">
+        <v>1959.9999999999998</v>
+      </c>
+      <c r="L1181" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1181" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1181" s="2">
+        <v>1959.9999999999998</v>
+      </c>
+      <c r="S1181" s="2">
+        <v>1959.9999999999998</v>
+      </c>
+      <c r="U1181" s="2">
+        <v>1959.9999999999998</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1182">
+        <v>40</v>
+      </c>
+      <c r="C1182" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1182" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1182" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1182" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1182">
+        <v>2.16</v>
+      </c>
+      <c r="H1182">
+        <v>700</v>
+      </c>
+      <c r="I1182" s="2">
+        <v>1512</v>
+      </c>
+      <c r="L1182" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1182" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1182" s="2">
+        <v>1512</v>
+      </c>
+      <c r="S1182" s="2">
+        <v>1512</v>
+      </c>
+      <c r="U1182" s="2">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1183">
+        <v>40</v>
+      </c>
+      <c r="C1183" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1183" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1183" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1183" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1183" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1183" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1183">
+        <v>5</v>
+      </c>
+      <c r="N1183">
+        <v>1083</v>
+      </c>
+      <c r="O1183" s="2">
+        <v>5415</v>
+      </c>
+      <c r="P1183" s="2">
+        <v>5415</v>
+      </c>
+      <c r="S1183" s="2">
+        <v>5415</v>
+      </c>
+      <c r="U1183" s="2">
+        <v>5415</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1184">
+        <v>40</v>
+      </c>
+      <c r="C1184" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1184" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1184" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1184" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1184">
+        <v>2.6</v>
+      </c>
+      <c r="H1184">
+        <v>200</v>
+      </c>
+      <c r="I1184" s="2">
+        <v>520</v>
+      </c>
+      <c r="J1184">
+        <v>5</v>
+      </c>
+      <c r="K1184">
+        <v>700</v>
+      </c>
+      <c r="L1184" s="2">
+        <v>3500</v>
+      </c>
+      <c r="O1184" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1184" s="2">
+        <v>4020</v>
+      </c>
+      <c r="S1184" s="2">
+        <v>4020</v>
+      </c>
+      <c r="U1184" s="2">
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1185">
+        <v>40</v>
+      </c>
+      <c r="C1185" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1185" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1185" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1185" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1185">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="H1185">
+        <v>200</v>
+      </c>
+      <c r="I1185" s="2">
+        <v>490.00000000000006</v>
+      </c>
+      <c r="L1185" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1185" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1185" s="2">
+        <v>490.00000000000006</v>
+      </c>
+      <c r="S1185" s="2">
+        <v>490.00000000000006</v>
+      </c>
+      <c r="U1185" s="2">
+        <v>490.00000000000006</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1186">
+        <v>40</v>
+      </c>
+      <c r="C1186" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1186" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1186" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1186" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1186">
+        <v>0.41</v>
+      </c>
+      <c r="H1186">
+        <v>900</v>
+      </c>
+      <c r="I1186" s="2">
+        <v>369</v>
+      </c>
+      <c r="L1186" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1186">
+        <v>0.5</v>
+      </c>
+      <c r="N1186">
+        <v>1083.33</v>
+      </c>
+      <c r="O1186" s="2">
+        <v>541.66499999999996</v>
+      </c>
+      <c r="P1186" s="2">
+        <v>910.66499999999996</v>
+      </c>
+      <c r="S1186" s="2">
+        <v>910.66499999999996</v>
+      </c>
+      <c r="U1186" s="2">
+        <v>910.66499999999996</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1187">
+        <v>40</v>
+      </c>
+      <c r="C1187" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1187" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1187" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1187" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1187">
+        <v>0.64</v>
+      </c>
+      <c r="H1187">
+        <v>300</v>
+      </c>
+      <c r="I1187" s="2">
+        <v>192</v>
+      </c>
+      <c r="L1187" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1187" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1187" s="2">
+        <v>192</v>
+      </c>
+      <c r="S1187" s="2">
+        <v>192</v>
+      </c>
+      <c r="U1187" s="2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1188">
+        <v>40</v>
+      </c>
+      <c r="C1188" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1188" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1188" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1188" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1188">
+        <v>2</v>
+      </c>
+      <c r="H1188">
+        <v>300</v>
+      </c>
+      <c r="I1188" s="2">
+        <v>600</v>
+      </c>
+      <c r="L1188" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1188" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1188" s="2">
+        <v>600</v>
+      </c>
+      <c r="S1188" s="2">
+        <v>600</v>
+      </c>
+      <c r="U1188" s="2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1189">
+        <v>40</v>
+      </c>
+      <c r="C1189" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1189" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1189" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1189" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1189">
+        <v>2.76</v>
+      </c>
+      <c r="H1189">
+        <v>300</v>
+      </c>
+      <c r="I1189" s="2">
+        <v>827.99999999999989</v>
+      </c>
+      <c r="L1189" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1189" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1189" s="2">
+        <v>827.99999999999989</v>
+      </c>
+      <c r="S1189" s="2">
+        <v>827.99999999999989</v>
+      </c>
+      <c r="U1189" s="2">
+        <v>827.99999999999989</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1190">
+        <v>40</v>
+      </c>
+      <c r="C1190" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1190" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1190" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1190" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1190">
+        <v>2.76</v>
+      </c>
+      <c r="H1190">
+        <v>100</v>
+      </c>
+      <c r="I1190" s="2">
+        <v>276</v>
+      </c>
+      <c r="L1190" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1190" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1190" s="2">
+        <v>276</v>
+      </c>
+      <c r="S1190" s="2">
+        <v>276</v>
+      </c>
+      <c r="U1190" s="2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1191">
+        <v>40</v>
+      </c>
+      <c r="C1191" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1191" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1191" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1191" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1191">
+        <v>3.08</v>
+      </c>
+      <c r="H1191">
+        <v>400</v>
+      </c>
+      <c r="I1191" s="2">
+        <v>1232</v>
+      </c>
+      <c r="L1191" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1191" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1191" s="2">
+        <v>1232</v>
+      </c>
+      <c r="Q1191" s="2">
+        <v>500</v>
+      </c>
+      <c r="S1191" s="2">
+        <v>1732</v>
+      </c>
+      <c r="U1191" s="2">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1192">
+        <v>40</v>
+      </c>
+      <c r="C1192" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1192" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1192" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1192" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1192" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1192">
+        <v>1</v>
+      </c>
+      <c r="K1192">
+        <v>250</v>
+      </c>
+      <c r="L1192" s="2">
+        <v>250</v>
+      </c>
+      <c r="O1192" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1192" s="2">
+        <v>250</v>
+      </c>
+      <c r="S1192" s="2">
+        <v>250</v>
+      </c>
+      <c r="U1192" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1193">
+        <v>40</v>
+      </c>
+      <c r="C1193" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1193" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1193" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1193" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1193" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1193">
+        <v>1</v>
+      </c>
+      <c r="K1193">
+        <v>750</v>
+      </c>
+      <c r="L1193" s="2">
+        <v>750</v>
+      </c>
+      <c r="O1193" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1193" s="2">
+        <v>750</v>
+      </c>
+      <c r="S1193" s="2">
+        <v>750</v>
+      </c>
+      <c r="U1193" s="2">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1194">
+        <v>40</v>
+      </c>
+      <c r="C1194" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1194" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1194" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1194" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1194" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1194">
+        <v>1</v>
+      </c>
+      <c r="K1194">
+        <v>1800</v>
+      </c>
+      <c r="L1194" s="2">
+        <v>1800</v>
+      </c>
+      <c r="O1194" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1194" s="2">
+        <v>1800</v>
+      </c>
+      <c r="S1194" s="2">
+        <v>1800</v>
+      </c>
+      <c r="U1194" s="2">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1195">
+        <v>40</v>
+      </c>
+      <c r="C1195" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1195" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1195" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1195" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1195">
+        <v>10.5</v>
+      </c>
+      <c r="H1195">
+        <v>250</v>
+      </c>
+      <c r="I1195" s="2">
+        <v>2625</v>
+      </c>
+      <c r="L1195" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1195" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1195" s="2">
+        <v>2625</v>
+      </c>
+      <c r="S1195" s="2">
+        <v>2625</v>
+      </c>
+      <c r="U1195" s="2">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1196">
+        <v>40</v>
+      </c>
+      <c r="C1196" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1196" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1196" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1196" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1196">
+        <v>3.8650000000000002</v>
+      </c>
+      <c r="H1196">
+        <v>700</v>
+      </c>
+      <c r="I1196" s="2">
+        <v>2705.5</v>
+      </c>
+      <c r="J1196">
+        <v>1</v>
+      </c>
+      <c r="K1196">
+        <v>400</v>
+      </c>
+      <c r="L1196" s="2">
+        <v>400</v>
+      </c>
+      <c r="O1196" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1196" s="2">
+        <v>3105.5</v>
+      </c>
+      <c r="S1196" s="2">
+        <v>3105.5</v>
+      </c>
+      <c r="U1196" s="2">
+        <v>3105.5</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1197">
+        <v>40</v>
+      </c>
+      <c r="C1197" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1197" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1197" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1197" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1197">
+        <v>3.8650000000000002</v>
+      </c>
+      <c r="H1197">
+        <v>700</v>
+      </c>
+      <c r="I1197" s="2">
+        <v>2705.5</v>
+      </c>
+      <c r="J1197">
+        <v>1</v>
+      </c>
+      <c r="K1197">
+        <v>400</v>
+      </c>
+      <c r="L1197" s="2">
+        <v>400</v>
+      </c>
+      <c r="O1197" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1197" s="2">
+        <v>3105.5</v>
+      </c>
+      <c r="S1197" s="2">
+        <v>3105.5</v>
+      </c>
+      <c r="U1197" s="2">
+        <v>3105.5</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1198">
+        <v>40</v>
+      </c>
+      <c r="C1198" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1198" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1198" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1198" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1198">
+        <v>1.8049999999999999</v>
+      </c>
+      <c r="H1198">
+        <v>700</v>
+      </c>
+      <c r="I1198" s="2">
+        <v>1263.5</v>
+      </c>
+      <c r="J1198">
+        <v>1</v>
+      </c>
+      <c r="K1198">
+        <v>200</v>
+      </c>
+      <c r="L1198" s="2">
+        <v>200</v>
+      </c>
+      <c r="O1198" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1198" s="2">
+        <v>1463.5</v>
+      </c>
+      <c r="S1198" s="2">
+        <v>1463.5</v>
+      </c>
+      <c r="U1198" s="2">
+        <v>1463.5</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1199">
+        <v>40</v>
+      </c>
+      <c r="C1199" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1199" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1199" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1199" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1199">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="H1199">
+        <v>700</v>
+      </c>
+      <c r="I1199" s="2">
+        <v>1624</v>
+      </c>
+      <c r="J1199">
+        <v>1</v>
+      </c>
+      <c r="K1199">
+        <v>200</v>
+      </c>
+      <c r="L1199" s="2">
+        <v>200</v>
+      </c>
+      <c r="O1199" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1199" s="2">
+        <v>1824</v>
+      </c>
+      <c r="S1199" s="2">
+        <v>1824</v>
+      </c>
+      <c r="U1199" s="2">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1200">
+        <v>40</v>
+      </c>
+      <c r="C1200" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1200" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1200" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1200" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1200">
+        <v>3.09</v>
+      </c>
+      <c r="H1200">
+        <v>700</v>
+      </c>
+      <c r="I1200" s="2">
+        <v>2163</v>
+      </c>
+      <c r="L1200" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1200" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1200" s="2">
+        <v>2163</v>
+      </c>
+      <c r="S1200" s="2">
+        <v>2163</v>
+      </c>
+      <c r="U1200" s="2">
+        <v>2163</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1201">
+        <v>40</v>
+      </c>
+      <c r="C1201" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1201" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1201" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1201" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1201" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1201">
+        <v>1</v>
+      </c>
+      <c r="K1201">
+        <v>750</v>
+      </c>
+      <c r="L1201" s="2">
+        <v>750</v>
+      </c>
+      <c r="O1201" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1201" s="2">
+        <v>750</v>
+      </c>
+      <c r="S1201" s="2">
+        <v>750</v>
+      </c>
+      <c r="U1201" s="2">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1202">
+        <v>40</v>
+      </c>
+      <c r="C1202" s="1">
+        <v>45568</v>
+      </c>
+      <c r="D1202" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1202" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1202" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1202" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1202" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1202">
+        <v>1</v>
+      </c>
+      <c r="N1202">
+        <v>5000</v>
+      </c>
+      <c r="O1202" s="2">
+        <v>5000</v>
+      </c>
+      <c r="P1202" s="2">
+        <v>5000</v>
+      </c>
+      <c r="S1202" s="2">
+        <v>5000</v>
+      </c>
+      <c r="U1202" s="2">
+        <v>5000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>